<commit_message>
Updated creatclient CredentialLogin method
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_MLY_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_MLY_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="39" activeTab="39"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="67" activeTab="70"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -82,8 +82,9 @@
     <sheet name="CombinedInvoice" sheetId="74" r:id="rId68"/>
     <sheet name="InvoiceMPL" sheetId="59" r:id="rId69"/>
     <sheet name="QuoteMPL" sheetId="60" r:id="rId70"/>
-    <sheet name="Agency Users" sheetId="11" r:id="rId71"/>
-    <sheet name="SSC Users" sheetId="12" r:id="rId72"/>
+    <sheet name="PurchaseOrderMPL" sheetId="75" r:id="rId71"/>
+    <sheet name="Agency Users" sheetId="11" r:id="rId72"/>
+    <sheet name="SSC Users" sheetId="12" r:id="rId73"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -95,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2857" uniqueCount="1549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3013" uniqueCount="1590">
   <si>
     <t>Description</t>
   </si>
@@ -4499,12 +4500,6 @@
     <t>2-2</t>
   </si>
   <si>
-    <t>2001_MarReg</t>
-  </si>
-  <si>
-    <t>March BAU Regression</t>
-  </si>
-  <si>
     <t>200120273</t>
   </si>
   <si>
@@ -4529,9 +4524,6 @@
     <t>2001701567</t>
   </si>
   <si>
-    <t>20019938</t>
-  </si>
-  <si>
     <t>2001401494</t>
   </si>
   <si>
@@ -4577,9 +4569,6 @@
     <t>2001_AutomationEmpy@gmail.com</t>
   </si>
   <si>
-    <t>20019905</t>
-  </si>
-  <si>
     <t>AUTOFILL</t>
   </si>
   <si>
@@ -4640,33 +4629,6 @@
     <t>GlobalVendor 29March2021 10:49:09</t>
   </si>
   <si>
-    <t>176.80</t>
-  </si>
-  <si>
-    <t>1,060.80</t>
-  </si>
-  <si>
-    <t>63.65</t>
-  </si>
-  <si>
-    <t>1124.45</t>
-  </si>
-  <si>
-    <t>88.40</t>
-  </si>
-  <si>
-    <t>2,210.00</t>
-  </si>
-  <si>
-    <t>132.60</t>
-  </si>
-  <si>
-    <t>2342.6</t>
-  </si>
-  <si>
-    <t>7,248.80</t>
-  </si>
-  <si>
     <t>4210000-01</t>
   </si>
   <si>
@@ -4719,9 +4681,6 @@
   </si>
   <si>
     <t>200118295</t>
-  </si>
-  <si>
-    <t>200118297</t>
   </si>
   <si>
     <t xml:space="preserve">2001401534
@@ -4747,6 +4706,171 @@
   </si>
   <si>
     <t>200118300</t>
+  </si>
+  <si>
+    <t>EC1008</t>
+  </si>
+  <si>
+    <t>EC1008-Senior Finance Executive</t>
+  </si>
+  <si>
+    <t>2001AutomationUser</t>
+  </si>
+  <si>
+    <t>20010351</t>
+  </si>
+  <si>
+    <t>2001_AutoClient 18April2021 17:54:17</t>
+  </si>
+  <si>
+    <t>110706</t>
+  </si>
+  <si>
+    <t>110706001</t>
+  </si>
+  <si>
+    <t>110706001001</t>
+  </si>
+  <si>
+    <t>AutoGlobalBrand 18April2021 17:54:17</t>
+  </si>
+  <si>
+    <t>AutoGlobalProduct 18April2021 17:54:17</t>
+  </si>
+  <si>
+    <t>126904</t>
+  </si>
+  <si>
+    <t>GlobalVendor 18April2021 18:56:58</t>
+  </si>
+  <si>
+    <t>175.64</t>
+  </si>
+  <si>
+    <t>1,053.84</t>
+  </si>
+  <si>
+    <t>63.23</t>
+  </si>
+  <si>
+    <t>1117.07</t>
+  </si>
+  <si>
+    <t>87.82</t>
+  </si>
+  <si>
+    <t>2,195.50</t>
+  </si>
+  <si>
+    <t>131.73</t>
+  </si>
+  <si>
+    <t>2327.23</t>
+  </si>
+  <si>
+    <t>7,201.24</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestAutomation2\GlobalTestSuiteAutomation\WppRegPack\MPLReports\Critical_Regression\Malaysia\2001\Print Job Order Confirmation-1.pdf</t>
+  </si>
+  <si>
+    <t>200110935</t>
+  </si>
+  <si>
+    <t>April BAU Regression</t>
+  </si>
+  <si>
+    <t>2001_APR Reg</t>
+  </si>
+  <si>
+    <t>200118410</t>
+  </si>
+  <si>
+    <t>5/19/2021</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>2001701659</t>
+  </si>
+  <si>
+    <t>2001401561</t>
+  </si>
+  <si>
+    <t>2001401562</t>
+  </si>
+  <si>
+    <t>2001401563</t>
+  </si>
+  <si>
+    <t>Single Payment Trans No</t>
+  </si>
+  <si>
+    <t>2001450992</t>
+  </si>
+  <si>
+    <t>Account Number</t>
+  </si>
+  <si>
+    <t>105723563101</t>
+  </si>
+  <si>
+    <t>200118414</t>
+  </si>
+  <si>
+    <t>Multiple Payment Trans No</t>
+  </si>
+  <si>
+    <t>2001450993</t>
+  </si>
+  <si>
+    <t>200118415</t>
+  </si>
+  <si>
+    <t>Foreign Payment Trans No</t>
+  </si>
+  <si>
+    <t>2001450994</t>
+  </si>
+  <si>
+    <t>200118416</t>
+  </si>
+  <si>
+    <t>200118417</t>
+  </si>
+  <si>
+    <t>Financeplus Malaysia (2001)</t>
+  </si>
+  <si>
+    <t>4/19/2021</t>
+  </si>
+  <si>
+    <t>4/1/2021</t>
+  </si>
+  <si>
+    <t>4/30/2021</t>
+  </si>
+  <si>
+    <t>2001607335</t>
+  </si>
+  <si>
+    <t>2001512726</t>
+  </si>
+  <si>
+    <t>JobNumber</t>
+  </si>
+  <si>
+    <t>1753101755</t>
+  </si>
+  <si>
+    <t>3rd Party Resource</t>
+  </si>
+  <si>
+    <t>PurchaseOrderMPL</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestAutomation2\GlobalTestSuiteAutomation\WppRegPack\MPLReports\Critical_Regression\Malaysia\2001\P_PurchaseOrder-4.pdf</t>
   </si>
 </sst>
 </file>
@@ -5031,7 +5155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5216,9 +5340,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -5508,7 +5629,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5814,7 +5935,7 @@
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6032,13 +6153,13 @@
         <v>2001</v>
       </c>
       <c r="C4">
-        <v>20019905</v>
+        <v>20019933</v>
       </c>
       <c r="D4" t="s">
         <v>990</v>
       </c>
       <c r="E4" t="s">
-        <v>1524</v>
+        <v>1511</v>
       </c>
       <c r="F4" t="s">
         <v>510</v>
@@ -6061,7 +6182,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:E18"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6110,7 +6231,7 @@
         <v>46</v>
       </c>
       <c r="E3" s="48">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -6127,7 +6248,7 @@
         <v>1108</v>
       </c>
       <c r="E4" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -6211,6 +6332,9 @@
       <c r="D9">
         <v>8</v>
       </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
@@ -6225,6 +6349,9 @@
       <c r="D10">
         <v>8</v>
       </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
@@ -6234,6 +6361,9 @@
       <c r="D11">
         <v>8</v>
       </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
@@ -6305,7 +6435,9 @@
       <c r="D16" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="19"/>
+      <c r="E16" s="19" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -6320,7 +6452,9 @@
       <c r="D17" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="19"/>
+      <c r="E17" s="19" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -6335,7 +6469,9 @@
       <c r="D18" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="19"/>
+      <c r="E18" s="19" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -6364,7 +6500,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6393,7 +6529,7 @@
         <v>1144</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>1489</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -6426,7 +6562,7 @@
         <v>1069</v>
       </c>
       <c r="C5" t="s">
-        <v>1490</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -6434,10 +6570,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>1493</v>
+        <v>1489</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>1493</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -6459,7 +6595,7 @@
         <v>1145</v>
       </c>
       <c r="C8" s="90" t="s">
-        <v>1491</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6547,7 +6683,7 @@
         <v>1141</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>1492</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -6558,7 +6694,7 @@
         <v>1141</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>1492</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -6569,7 +6705,7 @@
         <v>186</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>186</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6580,7 +6716,7 @@
         <v>1143</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>1143</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -6624,20 +6760,21 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" style="19" width="24.140625" collapsed="true"/>
     <col min="2" max="3" customWidth="true" style="19" width="23.140625" collapsed="true"/>
-    <col min="4" max="16384" style="19" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="19" width="28.7109375" collapsed="true"/>
+    <col min="5" max="16384" style="19" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>4</v>
       </c>
@@ -6647,8 +6784,11 @@
       <c r="C1" s="39" t="s">
         <v>1063</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="39">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>2</v>
       </c>
@@ -6658,8 +6798,11 @@
       <c r="C2" t="s">
         <v>1281</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>1282</v>
       </c>
@@ -6669,8 +6812,11 @@
       <c r="C3" s="40" t="s">
         <v>1063</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="40">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>182</v>
       </c>
@@ -6680,8 +6826,11 @@
       <c r="C4" s="40" t="s">
         <v>1141</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="48" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
         <v>54</v>
       </c>
@@ -6689,8 +6838,11 @@
       <c r="C5" t="s">
         <v>1069</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
         <v>15</v>
       </c>
@@ -6700,30 +6852,39 @@
       <c r="C6" s="40" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
         <v>45</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>1493</v>
+        <v>1489</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>1493</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1489</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>1493</v>
+        <v>1489</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>1493</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1489</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
         <v>47</v>
       </c>
@@ -6732,6 +6893,9 @@
       </c>
       <c r="C9" s="40" t="s">
         <v>1063</v>
+      </c>
+      <c r="D9" s="40">
+        <v>2001</v>
       </c>
     </row>
   </sheetData>
@@ -6747,8 +6911,8 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6764,8 +6928,8 @@
       <c r="B1" t="s">
         <v>1063</v>
       </c>
-      <c r="C1">
-        <v>2001</v>
+      <c r="C1" s="48" t="s">
+        <v>1461</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6776,7 +6940,7 @@
         <v>1144</v>
       </c>
       <c r="C2" t="s">
-        <v>1489</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -6820,7 +6984,7 @@
         <v>1069</v>
       </c>
       <c r="C6" t="s">
-        <v>1490</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -6831,7 +6995,7 @@
         <v>1338</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>1493</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6853,7 +7017,7 @@
         <v>1144</v>
       </c>
       <c r="C9" t="s">
-        <v>1489</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6941,7 +7105,7 @@
         <v>1141</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>1492</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -6952,7 +7116,7 @@
         <v>1141</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>1492</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6962,8 +7126,8 @@
       <c r="B19" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="C19" s="48" t="s">
-        <v>186</v>
+      <c r="C19" s="13" t="s">
+        <v>1535</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -6973,8 +7137,8 @@
       <c r="B20" t="s">
         <v>1143</v>
       </c>
-      <c r="C20" t="s">
-        <v>1143</v>
+      <c r="C20" s="46" t="s">
+        <v>1536</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -7018,7 +7182,7 @@
         <v>1338</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>1493</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -7029,7 +7193,7 @@
         <v>1339</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>1493</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -7040,7 +7204,7 @@
         <v>1146</v>
       </c>
       <c r="C26" t="s">
-        <v>1494</v>
+        <v>1490</v>
       </c>
     </row>
   </sheetData>
@@ -7544,39 +7708,41 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:FC91"/>
+  <dimension ref="A1:FE95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" customWidth="true" style="19" width="39.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="19" width="27.85546875" collapsed="true"/>
-    <col min="7" max="159" customWidth="true" style="19" width="32.0" collapsed="true"/>
-    <col min="160" max="16384" style="19" width="9.140625" collapsed="true"/>
+    <col min="1" max="7" customWidth="true" style="19" width="39.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="19" width="27.85546875" collapsed="true"/>
+    <col min="9" max="161" customWidth="true" style="19" width="32.0" collapsed="true"/>
+    <col min="162" max="16384" style="19" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>175</v>
       </c>
       <c r="B1" s="10">
         <v>2001</v>
       </c>
-      <c r="C1" s="10">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10">
+        <v>2001</v>
+      </c>
+      <c r="E1" s="10">
         <v>2011</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10">
         <v>2025</v>
       </c>
-      <c r="F1" s="10">
+      <c r="H1" s="10">
         <v>20234</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -7728,385 +7894,456 @@
       <c r="FA1" s="10"/>
       <c r="FB1" s="10"/>
       <c r="FC1" s="10"/>
-    </row>
-    <row r="2" spans="1:159" x14ac:dyDescent="0.25">
+      <c r="FD1" s="10"/>
+      <c r="FE1" s="10"/>
+    </row>
+    <row r="2" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>1481</v>
+        <v>1466</v>
       </c>
       <c r="C2" t="s">
+        <v>1466</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1478</v>
+      </c>
+      <c r="E2" t="s">
         <v>1460</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>1460</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>1409</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>1277</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>1107</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>1259</v>
       </c>
     </row>
-    <row r="3" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>182</v>
       </c>
       <c r="B3" t="s">
-        <v>1537</v>
+        <v>1538</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>1478</v>
       </c>
       <c r="D3" t="s">
+        <v>1524</v>
+      </c>
+      <c r="F3" t="s">
         <v>1464</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>1340</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>1148</v>
       </c>
     </row>
-    <row r="4" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>183</v>
       </c>
       <c r="B4" t="s">
-        <v>1533</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1475</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>1468</v>
+        <v>1563</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1520</v>
       </c>
       <c r="E4" t="s">
+        <v>1473</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>1466</v>
+      </c>
+      <c r="G4" t="s">
         <v>1367</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>1150</v>
       </c>
     </row>
-    <row r="5" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>199</v>
       </c>
       <c r="B5" t="s">
-        <v>1528</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1469</v>
-      </c>
-      <c r="D5">
+        <v>1557</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1515</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1467</v>
+      </c>
+      <c r="F5">
         <v>200120274</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>1360</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="H5" s="19" t="s">
         <v>1140</v>
       </c>
     </row>
-    <row r="6" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>710</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>1530</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>1470</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B6" t="s">
+        <v>1560</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>1517</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>1468</v>
+      </c>
+      <c r="G6" t="s">
         <v>1364</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>1157</v>
       </c>
     </row>
-    <row r="7" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>711</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>1529</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>1471</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B7" t="s">
+        <v>1559</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>1516</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>1469</v>
+      </c>
+      <c r="G7" t="s">
         <v>1361</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>1152</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>1152</v>
       </c>
     </row>
-    <row r="8" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>1020</v>
       </c>
       <c r="B8" t="s">
         <v>1432</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>1432</v>
       </c>
       <c r="E8" t="s">
+        <v>1432</v>
+      </c>
+      <c r="G8" t="s">
         <v>1141</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>1141</v>
       </c>
     </row>
-    <row r="9" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>1021</v>
       </c>
       <c r="B9" t="s">
         <v>1444</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>1444</v>
       </c>
       <c r="E9" t="s">
+        <v>1444</v>
+      </c>
+      <c r="G9" t="s">
         <v>995</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>995</v>
       </c>
     </row>
-    <row r="10" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>1022</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>1532</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1473</v>
+      <c r="B10" t="s">
+        <v>1562</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>1519</v>
       </c>
       <c r="E10" t="s">
+        <v>1471</v>
+      </c>
+      <c r="G10" t="s">
         <v>1366</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>1142</v>
       </c>
     </row>
-    <row r="11" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>1023</v>
       </c>
     </row>
-    <row r="12" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>1024</v>
       </c>
     </row>
-    <row r="13" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>970</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>1498</v>
-      </c>
-      <c r="C13" s="19" t="s">
+      <c r="B13" s="49" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C13" s="49"/>
+      <c r="D13" s="19" t="s">
+        <v>1494</v>
+      </c>
+      <c r="E13" s="19" t="s">
         <v>1434</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>1346</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>1316</v>
       </c>
     </row>
-    <row r="14" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>1025</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>1499</v>
-      </c>
-      <c r="C14" s="19" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>1495</v>
+      </c>
+      <c r="E14" s="19" t="s">
         <v>1433</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>1347</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
         <v>1317</v>
       </c>
     </row>
-    <row r="15" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>971</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>1506</v>
-      </c>
-      <c r="C15" s="19" t="s">
+      <c r="B15" s="49" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C15" s="49"/>
+      <c r="D15" s="19" t="s">
+        <v>1502</v>
+      </c>
+      <c r="E15" s="19" t="s">
         <v>1435</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>1348</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>1318</v>
       </c>
     </row>
-    <row r="16" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:161" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>1026</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>1507</v>
-      </c>
-      <c r="C16" s="19" t="s">
+        <v>1543</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>1503</v>
+      </c>
+      <c r="E16" s="19" t="s">
         <v>1436</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>1349</v>
       </c>
-      <c r="F16" t="s">
+      <c r="H16" t="s">
         <v>1319</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>972</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>1508</v>
-      </c>
-      <c r="C17" s="19" t="s">
+      <c r="B17" s="49" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C17" s="49"/>
+      <c r="D17" s="19" t="s">
+        <v>1504</v>
+      </c>
+      <c r="E17" s="19" t="s">
         <v>1437</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>1350</v>
       </c>
-      <c r="F17" t="s">
+      <c r="H17" t="s">
         <v>1320</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>1027</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>1509</v>
-      </c>
-      <c r="C18" s="19" t="s">
+        <v>1544</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>1505</v>
+      </c>
+      <c r="E18" s="19" t="s">
         <v>1438</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>1351</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>1321</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>1028</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>1029</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>187</v>
       </c>
       <c r="B21" t="s">
-        <v>1510</v>
-      </c>
-      <c r="C21" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C21"/>
+      <c r="D21" t="s">
+        <v>1506</v>
+      </c>
+      <c r="E21" t="s">
         <v>1439</v>
       </c>
-      <c r="D21"/>
-      <c r="E21" t="s">
+      <c r="F21"/>
+      <c r="G21" t="s">
         <v>1352</v>
       </c>
-      <c r="F21" t="s">
+      <c r="H21" t="s">
         <v>1322</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>1030</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>1031</v>
       </c>
       <c r="B23" t="s">
-        <v>1548</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1487</v>
+        <v>1578</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1534</v>
       </c>
       <c r="E23" t="s">
+        <v>1484</v>
+      </c>
+      <c r="G23" t="s">
         <v>1395</v>
       </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
         <v>1229</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F24" t="s">
+      <c r="H24" t="s">
         <v>1149</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>1032</v>
       </c>
       <c r="B25" t="s">
-        <v>1481</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1481</v>
-      </c>
-      <c r="D25"/>
+        <v>1478</v>
+      </c>
+      <c r="C25"/>
+      <c r="D25" t="s">
+        <v>1478</v>
+      </c>
       <c r="E25" t="s">
+        <v>1478</v>
+      </c>
+      <c r="F25"/>
+      <c r="G25" t="s">
         <v>1409</v>
       </c>
-      <c r="F25" t="s">
+      <c r="H25" t="s">
         <v>1277</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>1033</v>
       </c>
       <c r="B26" t="s">
         <v>201</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26"/>
+      <c r="D26" t="s">
         <v>201</v>
       </c>
-      <c r="D26"/>
       <c r="E26" t="s">
         <v>201</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26"/>
+      <c r="G26" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1034</v>
       </c>
@@ -8114,44 +8351,54 @@
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27"/>
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1035</v>
       </c>
-      <c r="B28" s="48" t="s">
-        <v>1531</v>
-      </c>
-      <c r="C28" s="48" t="s">
-        <v>1472</v>
-      </c>
-      <c r="D28"/>
-      <c r="E28" t="s">
+      <c r="B28" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C28"/>
+      <c r="D28" s="48" t="s">
+        <v>1518</v>
+      </c>
+      <c r="E28" s="48" t="s">
+        <v>1470</v>
+      </c>
+      <c r="F28"/>
+      <c r="G28" t="s">
         <v>1365</v>
       </c>
-      <c r="F28" t="s">
+      <c r="H28" t="s">
         <v>1158</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1036</v>
       </c>
       <c r="B29" t="s">
         <v>1427</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29"/>
+      <c r="D29" t="s">
         <v>1427</v>
       </c>
-      <c r="D29"/>
       <c r="E29" t="s">
+        <v>1427</v>
+      </c>
+      <c r="F29"/>
+      <c r="G29" t="s">
         <v>1404</v>
       </c>
-      <c r="F29" t="s">
+      <c r="H29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>958</v>
       </c>
@@ -8159,8 +8406,10 @@
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F30"/>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1037</v>
       </c>
@@ -8168,8 +8417,10 @@
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31"/>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1038</v>
       </c>
@@ -8177,8 +8428,10 @@
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F32"/>
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1039</v>
       </c>
@@ -8186,8 +8439,10 @@
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F33"/>
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1040</v>
       </c>
@@ -8195,8 +8450,10 @@
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F34"/>
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1041</v>
       </c>
@@ -8204,8 +8461,10 @@
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F35"/>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1042</v>
       </c>
@@ -8213,8 +8472,10 @@
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F36"/>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1043</v>
       </c>
@@ -8222,8 +8483,10 @@
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F37"/>
+      <c r="G37"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1044</v>
       </c>
@@ -8231,8 +8494,10 @@
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F38"/>
+      <c r="G38"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1045</v>
       </c>
@@ -8240,8 +8505,10 @@
       <c r="C39"/>
       <c r="D39"/>
       <c r="E39"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F39"/>
+      <c r="G39"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1046</v>
       </c>
@@ -8249,48 +8516,50 @@
       <c r="C40"/>
       <c r="D40"/>
       <c r="E40"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F40"/>
+      <c r="G40"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>1047</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="G41" s="19" t="s">
         <v>1354</v>
       </c>
-      <c r="F41" s="19" t="s">
+      <c r="H41" s="19" t="s">
         <v>1277</v>
       </c>
-      <c r="G41" t="s">
+      <c r="I41" t="s">
         <v>1107</v>
       </c>
-      <c r="H41" t="s">
+      <c r="J41" t="s">
         <v>1107</v>
       </c>
-      <c r="I41" t="s">
+      <c r="K41" t="s">
         <v>1263</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>1197</v>
       </c>
-      <c r="E42" s="19" t="s">
+      <c r="G42" s="19" t="s">
         <v>1392</v>
       </c>
-      <c r="F42" s="19" t="s">
+      <c r="H42" s="19" t="s">
         <v>1279</v>
       </c>
-      <c r="G42" s="19" t="s">
+      <c r="I42" s="19" t="s">
         <v>1198</v>
       </c>
-      <c r="H42" s="19" t="s">
+      <c r="J42" s="19" t="s">
         <v>1255</v>
       </c>
-      <c r="I42" t="s">
+      <c r="K42" t="s">
         <v>1259</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1048</v>
       </c>
@@ -8298,8 +8567,10 @@
       <c r="C43"/>
       <c r="D43"/>
       <c r="E43"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F43"/>
+      <c r="G43"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1049</v>
       </c>
@@ -8307,38 +8578,40 @@
       <c r="C44"/>
       <c r="D44"/>
       <c r="E44"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F44"/>
+      <c r="G44"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>1050</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>1051</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>1052</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>1054</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>1055</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1056</v>
       </c>
@@ -8346,8 +8619,10 @@
       <c r="C51"/>
       <c r="D51"/>
       <c r="E51"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F51"/>
+      <c r="G51"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1057</v>
       </c>
@@ -8355,8 +8630,10 @@
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F52"/>
+      <c r="G52"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1058</v>
       </c>
@@ -8364,8 +8641,10 @@
       <c r="C53"/>
       <c r="D53"/>
       <c r="E53"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F53"/>
+      <c r="G53"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1059</v>
       </c>
@@ -8373,8 +8652,10 @@
       <c r="C54"/>
       <c r="D54"/>
       <c r="E54"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F54"/>
+      <c r="G54"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1060</v>
       </c>
@@ -8382,8 +8663,10 @@
       <c r="C55"/>
       <c r="D55"/>
       <c r="E55"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F55"/>
+      <c r="G55"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1061</v>
       </c>
@@ -8391,8 +8674,10 @@
       <c r="C56"/>
       <c r="D56"/>
       <c r="E56"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F56"/>
+      <c r="G56"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1062</v>
       </c>
@@ -8400,324 +8685,396 @@
       <c r="C57"/>
       <c r="D57"/>
       <c r="E57"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F57"/>
+      <c r="G57"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>248</v>
       </c>
       <c r="B58" t="s">
-        <v>1484</v>
-      </c>
-      <c r="C58" t="s">
-        <v>1484</v>
-      </c>
-      <c r="D58"/>
+        <v>1481</v>
+      </c>
+      <c r="C58"/>
+      <c r="D58" t="s">
+        <v>1481</v>
+      </c>
       <c r="E58" t="s">
+        <v>1481</v>
+      </c>
+      <c r="F58"/>
+      <c r="G58" t="s">
         <v>1403</v>
       </c>
-      <c r="F58" t="s">
+      <c r="H58" t="s">
         <v>1151</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>1072</v>
       </c>
       <c r="B59" t="s">
         <v>286</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59"/>
+      <c r="D59" t="s">
         <v>286</v>
       </c>
-      <c r="D59"/>
       <c r="E59" t="s">
         <v>286</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59"/>
+      <c r="G59" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H59" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>1131</v>
       </c>
       <c r="B60" t="s">
-        <v>1544</v>
-      </c>
-      <c r="C60" t="s">
         <v>1278</v>
       </c>
-      <c r="D60"/>
+      <c r="C60"/>
+      <c r="D60" t="s">
+        <v>1530</v>
+      </c>
       <c r="E60" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F60"/>
+      <c r="G60" t="s">
         <v>1410</v>
       </c>
-      <c r="F60" t="s">
+      <c r="H60" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>1132</v>
       </c>
       <c r="B61" t="s">
-        <v>1545</v>
-      </c>
-      <c r="C61" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C61"/>
+      <c r="D61" t="s">
+        <v>1531</v>
+      </c>
+      <c r="E61" t="s">
         <v>1278</v>
       </c>
-      <c r="D61"/>
-      <c r="E61" t="s">
+      <c r="F61"/>
+      <c r="G61" t="s">
         <v>1411</v>
       </c>
-      <c r="F61" t="s">
+      <c r="H61" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1153</v>
       </c>
       <c r="B62" t="s">
         <v>1284</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62"/>
+      <c r="D62" t="s">
         <v>1284</v>
       </c>
-      <c r="D62"/>
       <c r="E62" t="s">
         <v>1284</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62"/>
+      <c r="G62" t="s">
         <v>1284</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H62" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>1154</v>
       </c>
-      <c r="B63" s="96" t="s">
+      <c r="B63" t="s">
         <v>1155</v>
       </c>
-      <c r="C63" s="96" t="s">
+      <c r="C63"/>
+      <c r="D63" s="96" t="s">
         <v>1155</v>
       </c>
-      <c r="D63"/>
-      <c r="E63" t="s">
+      <c r="E63" s="96" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F63"/>
+      <c r="G63" t="s">
         <v>1363</v>
       </c>
-      <c r="F63" t="s">
+      <c r="H63" t="s">
         <v>1155</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>1156</v>
       </c>
-      <c r="B64" s="96" t="s">
+      <c r="B64" t="s">
         <v>1155</v>
       </c>
-      <c r="C64" s="96" t="s">
+      <c r="C64"/>
+      <c r="D64" s="96" t="s">
         <v>1155</v>
       </c>
-      <c r="D64"/>
-      <c r="E64" t="s">
+      <c r="E64" s="96" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F64"/>
+      <c r="G64" t="s">
         <v>1363</v>
       </c>
-      <c r="F64" t="s">
+      <c r="H64" t="s">
         <v>1155</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1159</v>
       </c>
       <c r="B65" t="s">
-        <v>1530</v>
-      </c>
-      <c r="C65" t="s">
-        <v>1470</v>
-      </c>
-      <c r="D65"/>
+        <v>1560</v>
+      </c>
+      <c r="C65"/>
+      <c r="D65" t="s">
+        <v>1517</v>
+      </c>
       <c r="E65" t="s">
+        <v>1468</v>
+      </c>
+      <c r="F65"/>
+      <c r="G65" t="s">
         <v>1364</v>
       </c>
-      <c r="F65" t="s">
+      <c r="H65" t="s">
         <v>1157</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1196</v>
       </c>
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66"/>
-      <c r="E66" t="s">
+      <c r="E66"/>
+      <c r="F66"/>
+      <c r="G66" t="s">
         <v>1391</v>
       </c>
-      <c r="F66" t="s">
+      <c r="H66" t="s">
         <v>1260</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1199</v>
       </c>
       <c r="B67" t="s">
-        <v>1539</v>
-      </c>
-      <c r="C67" t="s">
-        <v>1479</v>
-      </c>
-      <c r="D67"/>
+        <v>1571</v>
+      </c>
+      <c r="C67"/>
+      <c r="D67" t="s">
+        <v>1526</v>
+      </c>
       <c r="E67" t="s">
+        <v>1476</v>
+      </c>
+      <c r="F67"/>
+      <c r="G67" t="s">
         <v>1393</v>
       </c>
-      <c r="F67" t="s">
+      <c r="H67" t="s">
         <v>1257</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1200</v>
       </c>
       <c r="B68" t="s">
-        <v>1538</v>
-      </c>
-      <c r="C68" t="s">
-        <v>1477</v>
-      </c>
-      <c r="D68"/>
+        <v>1564</v>
+      </c>
+      <c r="C68"/>
+      <c r="D68" t="s">
+        <v>1525</v>
+      </c>
       <c r="E68" t="s">
+        <v>1474</v>
+      </c>
+      <c r="F68"/>
+      <c r="G68" t="s">
         <v>1392</v>
       </c>
-      <c r="F68" t="s">
+      <c r="H68" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1201</v>
       </c>
       <c r="B69" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C69"/>
+      <c r="D69" t="s">
         <v>1460</v>
       </c>
-      <c r="C69" t="s">
+      <c r="E69" t="s">
         <v>1460</v>
       </c>
-      <c r="D69"/>
-      <c r="E69" t="s">
+      <c r="F69"/>
+      <c r="G69" t="s">
         <v>1354</v>
       </c>
-      <c r="F69" t="s">
+      <c r="H69" t="s">
         <v>1259</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>1246</v>
       </c>
       <c r="B70" t="s">
         <v>1288</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70"/>
+      <c r="D70" t="s">
         <v>1288</v>
       </c>
-      <c r="D70"/>
       <c r="E70" t="s">
         <v>1288</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70"/>
+      <c r="G70" t="s">
         <v>1288</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H70" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1247</v>
       </c>
-      <c r="B71" t="s">
-        <v>1541</v>
+      <c r="B71" s="48" t="s">
+        <v>1564</v>
       </c>
       <c r="C71"/>
-      <c r="D71"/>
-      <c r="E71" t="s">
+      <c r="D71" t="s">
+        <v>1527</v>
+      </c>
+      <c r="E71"/>
+      <c r="F71"/>
+      <c r="G71" t="s">
         <v>1412</v>
       </c>
-      <c r="F71" t="s">
+      <c r="H71" t="s">
         <v>1248</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1249</v>
       </c>
       <c r="B72" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="C72"/>
-      <c r="D72"/>
-      <c r="E72" t="s">
+      <c r="D72" t="s">
+        <v>1466</v>
+      </c>
+      <c r="E72"/>
+      <c r="F72"/>
+      <c r="G72" t="s">
         <v>1409</v>
       </c>
-      <c r="F72" t="s">
+      <c r="H72" t="s">
         <v>1107</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>1253</v>
       </c>
       <c r="B73" t="s">
-        <v>1542</v>
-      </c>
-      <c r="C73" t="s">
-        <v>1482</v>
-      </c>
-      <c r="D73"/>
+        <v>1566</v>
+      </c>
+      <c r="C73"/>
+      <c r="D73" t="s">
+        <v>1528</v>
+      </c>
       <c r="E73" t="s">
+        <v>1479</v>
+      </c>
+      <c r="F73"/>
+      <c r="G73" t="s">
         <v>1413</v>
       </c>
-      <c r="F73" t="s">
+      <c r="H73" t="s">
         <v>1279</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1254</v>
       </c>
       <c r="B74" t="s">
-        <v>1468</v>
-      </c>
-      <c r="C74" t="s">
-        <v>1481</v>
-      </c>
-      <c r="D74"/>
+        <v>1464</v>
+      </c>
+      <c r="C74"/>
+      <c r="D74" t="s">
+        <v>1466</v>
+      </c>
       <c r="E74" t="s">
+        <v>1478</v>
+      </c>
+      <c r="F74"/>
+      <c r="G74" t="s">
         <v>1409</v>
       </c>
-      <c r="F74" t="s">
+      <c r="H74" t="s">
         <v>1277</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>1256</v>
       </c>
       <c r="B75" t="s">
-        <v>1543</v>
-      </c>
-      <c r="C75" t="s">
-        <v>1483</v>
-      </c>
-      <c r="D75"/>
+        <v>1577</v>
+      </c>
+      <c r="C75"/>
+      <c r="D75" t="s">
+        <v>1529</v>
+      </c>
       <c r="E75" t="s">
+        <v>1480</v>
+      </c>
+      <c r="F75"/>
+      <c r="G75" t="s">
         <v>1414</v>
       </c>
-      <c r="F75" t="s">
+      <c r="H75" t="s">
         <v>1280</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>1261</v>
       </c>
@@ -8725,187 +9082,261 @@
       <c r="C76"/>
       <c r="D76"/>
       <c r="E76"/>
-      <c r="F76" t="s">
+      <c r="F76"/>
+      <c r="G76"/>
+      <c r="H76" t="s">
         <v>1262</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
         <v>1264</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>1265</v>
       </c>
-      <c r="F78"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H78"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
         <v>1266</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
         <v>1267</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="19" t="s">
         <v>1268</v>
       </c>
-      <c r="G81" t="s">
+      <c r="I81" t="s">
         <v>1107</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">
         <v>1269</v>
       </c>
-      <c r="G82" t="s">
+      <c r="I82" t="s">
         <v>1248</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1273</v>
       </c>
       <c r="B83" t="s">
-        <v>1546</v>
-      </c>
-      <c r="C83" t="s">
-        <v>1478</v>
-      </c>
-      <c r="D83"/>
+        <v>1565</v>
+      </c>
+      <c r="C83"/>
+      <c r="D83" t="s">
+        <v>1532</v>
+      </c>
       <c r="E83" t="s">
+        <v>1475</v>
+      </c>
+      <c r="F83"/>
+      <c r="G83" t="s">
         <v>1408</v>
       </c>
-      <c r="F83" t="s">
+      <c r="H83" t="s">
         <v>1255</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1274</v>
       </c>
       <c r="B84" t="s">
-        <v>1481</v>
-      </c>
-      <c r="C84" t="s">
+        <v>1460</v>
+      </c>
+      <c r="C84"/>
+      <c r="D84" t="s">
+        <v>1478</v>
+      </c>
+      <c r="E84" t="s">
         <v>1464</v>
       </c>
-      <c r="D84"/>
-      <c r="E84" t="s">
+      <c r="F84"/>
+      <c r="G84" t="s">
         <v>1406</v>
       </c>
-      <c r="F84" t="s">
+      <c r="H84" t="s">
         <v>1107</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1275</v>
       </c>
       <c r="B85" t="s">
-        <v>1547</v>
-      </c>
-      <c r="C85" t="s">
-        <v>1480</v>
-      </c>
-      <c r="D85"/>
+        <v>1574</v>
+      </c>
+      <c r="C85"/>
+      <c r="D85" t="s">
+        <v>1533</v>
+      </c>
       <c r="E85" t="s">
+        <v>1477</v>
+      </c>
+      <c r="F85"/>
+      <c r="G85" t="s">
         <v>1407</v>
       </c>
-      <c r="F85" t="s">
+      <c r="H85" t="s">
         <v>1276</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1285</v>
       </c>
       <c r="B86" t="s">
-        <v>1534</v>
-      </c>
-      <c r="C86" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C86"/>
+      <c r="D86" t="s">
+        <v>1521</v>
+      </c>
+      <c r="E86" t="s">
         <v>1278</v>
       </c>
-      <c r="D86"/>
-      <c r="E86" t="s">
+      <c r="F86"/>
+      <c r="G86" t="s">
         <v>1399</v>
       </c>
-      <c r="F86" t="s">
+      <c r="H86" t="s">
         <v>1287</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1289</v>
       </c>
       <c r="B87" t="s">
-        <v>1535</v>
-      </c>
-      <c r="C87" t="s">
-        <v>1488</v>
-      </c>
-      <c r="D87"/>
+        <v>1584</v>
+      </c>
+      <c r="C87"/>
+      <c r="D87" t="s">
+        <v>1522</v>
+      </c>
       <c r="E87" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F87"/>
+      <c r="G87" t="s">
         <v>1400</v>
       </c>
-      <c r="F87" t="s">
+      <c r="H87" t="s">
         <v>1290</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1291</v>
       </c>
       <c r="B88" t="s">
-        <v>1536</v>
-      </c>
-      <c r="C88" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C88"/>
+      <c r="D88" t="s">
+        <v>1523</v>
+      </c>
+      <c r="E88" t="s">
         <v>1278</v>
       </c>
-      <c r="D88"/>
-      <c r="E88" t="s">
+      <c r="F88"/>
+      <c r="G88" t="s">
         <v>1401</v>
       </c>
-      <c r="F88" t="s">
+      <c r="H88" t="s">
         <v>1292</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1323</v>
       </c>
       <c r="B89" t="s">
         <v>510</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89"/>
+      <c r="D89" t="s">
         <v>510</v>
       </c>
-      <c r="D89"/>
       <c r="E89" t="s">
         <v>510</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F89"/>
+      <c r="G89" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H89" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
         <v>1334</v>
       </c>
-      <c r="E90" t="s">
+      <c r="G90" t="s">
         <v>1341</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>1511</v>
+        <v>1507</v>
       </c>
       <c r="B91" t="s">
-        <v>1512</v>
+        <v>1546</v>
+      </c>
+      <c r="C91"/>
+      <c r="D91" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>1567</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1575</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1589</v>
       </c>
     </row>
   </sheetData>
@@ -11004,7 +11435,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11095,7 +11526,7 @@
         <v>1402</v>
       </c>
       <c r="D6" s="92" t="s">
-        <v>1495</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -11140,7 +11571,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11198,7 +11629,7 @@
         <v>250</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -11243,7 +11674,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11507,7 +11938,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11640,16 +12071,16 @@
         <v>2001</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>1495</v>
+        <v>1489</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>1495</v>
+        <v>1489</v>
       </c>
       <c r="E6" t="s">
-        <v>1466</v>
+        <v>1559</v>
       </c>
       <c r="F6" t="s">
-        <v>1467</v>
+        <v>1558</v>
       </c>
     </row>
   </sheetData>
@@ -11821,10 +12252,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11835,7 +12266,7 @@
     <col min="4" max="16384" style="19" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>4</v>
       </c>
@@ -11855,15 +12286,15 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="F2" s="48" t="s">
-        <v>1460</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
@@ -11883,12 +12314,12 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>970</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>205</v>
       </c>
@@ -11908,13 +12339,19 @@
         <v>510</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>1251</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>1538</v>
-      </c>
+      <c r="F6" s="48" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="48"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13983,8 +14420,8 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14024,8 +14461,8 @@
       <c r="E2">
         <v>202522371</v>
       </c>
-      <c r="F2" s="48" t="s">
-        <v>1481</v>
+      <c r="F2">
+        <v>200120271</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -14080,8 +14517,8 @@
       <c r="E6">
         <v>2025401646</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>1546</v>
+      <c r="F6" s="48" t="s">
+        <v>1565</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -14162,7 +14599,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C7" sqref="A7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14191,7 +14628,7 @@
         <v>1409</v>
       </c>
       <c r="C2" s="48" t="s">
-        <v>1468</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -14228,8 +14665,8 @@
       <c r="B6" s="19" t="s">
         <v>1413</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>1542</v>
+      <c r="C6" s="48" t="s">
+        <v>1566</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -14237,6 +14674,9 @@
         <v>1252</v>
       </c>
       <c r="B7" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>257</v>
       </c>
     </row>
@@ -14737,7 +15177,7 @@
         <v>1394</v>
       </c>
       <c r="C5" s="84" t="s">
-        <v>1495</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -14816,7 +15256,7 @@
         <v>1394</v>
       </c>
       <c r="C3" s="84" t="s">
-        <v>1495</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -14914,7 +15354,7 @@
         <v>1394</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>1495</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -14957,10 +15397,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14971,7 +15411,7 @@
     <col min="4" max="4" customWidth="true" style="1" width="33.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
@@ -14982,7 +15422,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -14993,7 +15433,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>54</v>
       </c>
@@ -15004,7 +15444,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -15015,7 +15455,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
@@ -15026,7 +15466,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>975</v>
       </c>
@@ -15037,7 +15477,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>56</v>
       </c>
@@ -15048,7 +15488,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>57</v>
       </c>
@@ -15059,7 +15499,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
@@ -15070,7 +15510,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>53</v>
       </c>
@@ -15081,7 +15521,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
@@ -15092,7 +15532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>17</v>
       </c>
@@ -15103,7 +15543,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
@@ -15116,8 +15556,11 @@
       <c r="D13" s="4" t="s">
         <v>1427</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="4" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>58</v>
       </c>
@@ -15130,15 +15573,18 @@
       <c r="D14" s="21" t="s">
         <v>1428</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="21" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>11</v>
       </c>
@@ -15320,7 +15766,7 @@
         <v>916</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>1496</v>
+        <v>1492</v>
       </c>
       <c r="C9" s="48" t="s">
         <v>1342</v>
@@ -15334,7 +15780,7 @@
         <v>918</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>1497</v>
+        <v>1493</v>
       </c>
       <c r="C10" s="48" t="s">
         <v>1343</v>
@@ -15552,10 +15998,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1500</v>
+        <v>1496</v>
       </c>
       <c r="B29" t="s">
-        <v>1503</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -15563,20 +16009,20 @@
         <v>1206</v>
       </c>
       <c r="B30" t="s">
-        <v>1504</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B31" t="s">
         <v>1501</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1505</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1502</v>
+        <v>1498</v>
       </c>
       <c r="B32" t="s">
         <v>509</v>
@@ -16350,7 +16796,7 @@
         <v>266</v>
       </c>
       <c r="G4" t="s">
-        <v>1485</v>
+        <v>1482</v>
       </c>
       <c r="H4" s="48" t="s">
         <v>961</v>
@@ -16363,7 +16809,7 @@
         <v>266</v>
       </c>
       <c r="M4" t="s">
-        <v>1486</v>
+        <v>1483</v>
       </c>
       <c r="N4" s="48" t="s">
         <v>962</v>
@@ -16603,7 +17049,88 @@
         <v>1461</v>
       </c>
       <c r="B5" t="s">
-        <v>1548</v>
+        <v>1578</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1579</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1582</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1583</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1580</v>
+      </c>
+      <c r="J5" t="s">
+        <v>266</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1482</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1232</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1233</v>
+      </c>
+      <c r="O5" t="s">
+        <v>1424</v>
+      </c>
+      <c r="P5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>1121</v>
+      </c>
+      <c r="R5" t="s">
+        <v>1234</v>
+      </c>
+      <c r="S5" t="s">
+        <v>1583</v>
+      </c>
+      <c r="T5" t="s">
+        <v>1580</v>
+      </c>
+      <c r="U5" t="s">
+        <v>266</v>
+      </c>
+      <c r="V5" t="s">
+        <v>1483</v>
+      </c>
+      <c r="W5" t="s">
+        <v>1235</v>
+      </c>
+      <c r="X5" t="s">
+        <v>1232</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>1233</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>1424</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>1234</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>1121</v>
       </c>
     </row>
   </sheetData>
@@ -16700,7 +17227,7 @@
   <dimension ref="A1:AP5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16978,7 +17505,7 @@
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2001</v>
+        <v>201</v>
       </c>
       <c r="C4" t="s">
         <v>1454</v>
@@ -17019,13 +17546,13 @@
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2011</v>
+        <v>2001</v>
       </c>
       <c r="C5" t="s">
-        <v>1522</v>
+        <v>1509</v>
       </c>
       <c r="D5" t="s">
-        <v>1525</v>
+        <v>1512</v>
       </c>
       <c r="E5">
         <v>6</v>
@@ -17034,10 +17561,10 @@
         <v>1000</v>
       </c>
       <c r="G5" t="s">
-        <v>1523</v>
+        <v>1510</v>
       </c>
       <c r="H5" t="s">
-        <v>1526</v>
+        <v>1513</v>
       </c>
       <c r="I5">
         <v>25</v>
@@ -17046,10 +17573,10 @@
         <v>500</v>
       </c>
       <c r="K5" t="s">
-        <v>1524</v>
+        <v>1511</v>
       </c>
       <c r="L5" t="s">
-        <v>1527</v>
+        <v>1514</v>
       </c>
       <c r="M5">
         <v>10</v>
@@ -17739,7 +18266,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17812,8 +18339,8 @@
       <c r="A4" s="48" t="s">
         <v>1461</v>
       </c>
-      <c r="K4" s="98" t="s">
-        <v>1476</v>
+      <c r="K4">
+        <v>20019933</v>
       </c>
     </row>
   </sheetData>
@@ -18452,10 +18979,10 @@
         <v>1173</v>
       </c>
       <c r="D5" t="s">
-        <v>1513</v>
+        <v>1547</v>
       </c>
       <c r="E5" t="s">
-        <v>1514</v>
+        <v>1548</v>
       </c>
       <c r="F5" t="s">
         <v>1116</v>
@@ -18464,13 +18991,13 @@
         <v>1118</v>
       </c>
       <c r="H5" t="s">
-        <v>1515</v>
+        <v>1549</v>
       </c>
       <c r="I5" t="s">
         <v>1121</v>
       </c>
       <c r="J5" t="s">
-        <v>1516</v>
+        <v>1550</v>
       </c>
       <c r="K5" t="s">
         <v>1463</v>
@@ -18479,10 +19006,10 @@
         <v>1178</v>
       </c>
       <c r="M5" t="s">
-        <v>1517</v>
+        <v>1551</v>
       </c>
       <c r="N5" t="s">
-        <v>1518</v>
+        <v>1552</v>
       </c>
       <c r="O5" t="s">
         <v>1116</v>
@@ -18491,19 +19018,19 @@
         <v>1118</v>
       </c>
       <c r="Q5" t="s">
-        <v>1519</v>
+        <v>1553</v>
       </c>
       <c r="R5" t="s">
         <v>1121</v>
       </c>
       <c r="S5" t="s">
-        <v>1520</v>
+        <v>1554</v>
       </c>
       <c r="T5" t="s">
         <v>201</v>
       </c>
       <c r="U5" t="s">
-        <v>1521</v>
+        <v>1555</v>
       </c>
       <c r="V5" t="s">
         <v>1118</v>
@@ -18567,6 +19094,165 @@
 </file>
 
 <file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="21.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1585</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="K1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>1128</v>
+      </c>
+      <c r="M1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N1" t="s">
+        <v>118</v>
+      </c>
+      <c r="O1" t="s">
+        <v>190</v>
+      </c>
+      <c r="P1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="R1" t="s">
+        <v>121</v>
+      </c>
+      <c r="S1" t="s">
+        <v>122</v>
+      </c>
+      <c r="T1" t="s">
+        <v>191</v>
+      </c>
+      <c r="U1" t="s">
+        <v>78</v>
+      </c>
+      <c r="V1" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1513</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1155</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1155</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -18710,7 +19396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>

</xml_diff>

<commit_message>
Updated Date format and MPLs
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_MLY_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_MLY_REGRESSION.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestAutomation2\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestSuite\branches\bau_environment\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B31749-FE85-4688-82F6-9463C8B1C2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="67" activeTab="70"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3013" uniqueCount="1590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3156" uniqueCount="1634">
   <si>
     <t>Description</t>
   </si>
@@ -4461,9 +4462,6 @@
     <t>Global Regerssion</t>
   </si>
   <si>
-    <t>APAC - MYS - 2001-Financeplus Malaysia</t>
-  </si>
-  <si>
     <t>1099050-02</t>
   </si>
   <si>
@@ -4744,33 +4742,6 @@
     <t>GlobalVendor 18April2021 18:56:58</t>
   </si>
   <si>
-    <t>175.64</t>
-  </si>
-  <si>
-    <t>1,053.84</t>
-  </si>
-  <si>
-    <t>63.23</t>
-  </si>
-  <si>
-    <t>1117.07</t>
-  </si>
-  <si>
-    <t>87.82</t>
-  </si>
-  <si>
-    <t>2,195.50</t>
-  </si>
-  <si>
-    <t>131.73</t>
-  </si>
-  <si>
-    <t>2327.23</t>
-  </si>
-  <si>
-    <t>7,201.24</t>
-  </si>
-  <si>
     <t>C:\GlobalTestAutomation2\GlobalTestSuiteAutomation\WppRegPack\MPLReports\Critical_Regression\Malaysia\2001\Print Job Order Confirmation-1.pdf</t>
   </si>
   <si>
@@ -4843,40 +4814,206 @@
     <t>Financeplus Malaysia (2001)</t>
   </si>
   <si>
-    <t>4/19/2021</t>
-  </si>
-  <si>
-    <t>4/1/2021</t>
-  </si>
-  <si>
-    <t>4/30/2021</t>
-  </si>
-  <si>
-    <t>2001607335</t>
-  </si>
-  <si>
     <t>2001512726</t>
   </si>
   <si>
     <t>JobNumber</t>
   </si>
   <si>
-    <t>1753101755</t>
-  </si>
-  <si>
-    <t>3rd Party Resource</t>
-  </si>
-  <si>
     <t>PurchaseOrderMPL</t>
   </si>
   <si>
     <t>C:\GlobalTestAutomation2\GlobalTestSuiteAutomation\WppRegPack\MPLReports\Critical_Regression\Malaysia\2001\P_PurchaseOrder-4.pdf</t>
+  </si>
+  <si>
+    <t>APAC - MYS - 2001 - Financeplus Malaysia</t>
+  </si>
+  <si>
+    <t>111101</t>
+  </si>
+  <si>
+    <t>2001_AutoClient 13July2021 15:46:18</t>
+  </si>
+  <si>
+    <t>111101001</t>
+  </si>
+  <si>
+    <t>AutoGlobalBrand 13July2021 15:46:18</t>
+  </si>
+  <si>
+    <t>AutoGlobalProduct 13July2021 15:46:18</t>
+  </si>
+  <si>
+    <t>111101001001</t>
+  </si>
+  <si>
+    <t>Branch Name</t>
+  </si>
+  <si>
+    <t>127600</t>
+  </si>
+  <si>
+    <t>173.71</t>
+  </si>
+  <si>
+    <t>1,042.26</t>
+  </si>
+  <si>
+    <t>62.54</t>
+  </si>
+  <si>
+    <t>1104.8</t>
+  </si>
+  <si>
+    <t>86.86</t>
+  </si>
+  <si>
+    <t>2,171.50</t>
+  </si>
+  <si>
+    <t>130.29</t>
+  </si>
+  <si>
+    <t>2301.79</t>
+  </si>
+  <si>
+    <t>7,122.31</t>
+  </si>
+  <si>
+    <t>200118894</t>
+  </si>
+  <si>
+    <t>13-07-2021</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>2001607810</t>
+  </si>
+  <si>
+    <t>200120277</t>
+  </si>
+  <si>
+    <t>200120278</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>Timesheet Job No</t>
+  </si>
+  <si>
+    <t>Timesheet Hours</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>2001701783</t>
+  </si>
+  <si>
+    <t>Expense Description</t>
+  </si>
+  <si>
+    <t>Expenses 13July2021 22:39:49</t>
+  </si>
+  <si>
+    <t>200110968</t>
+  </si>
+  <si>
+    <t>200118900</t>
+  </si>
+  <si>
+    <t>13-08-2021</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestSuite\branches\bau_environment\WppRegPack\MPLReports\Critical_Regression\Malaysia\2001\PaymentSelection-2.pdf</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestSuite\branches\bau_environment\WppRegPack\MPLReports\Critical_Regression\Malaysia\2001\P_PurchaseOrder-1.pdf</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestSuite\branches\bau_environment\WppRegPack\MPLReports\Critical_Regression\Malaysia\2001\Print Invoice Editing-8.pdf</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestSuite\branches\bau_environment\WppRegPack\MPLReports\Critical_Regression\Malaysia\2001\Print Job Invoice-1.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001401678
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001401678
+</t>
+  </si>
+  <si>
+    <t>2001451072</t>
+  </si>
+  <si>
+    <t>200118903</t>
+  </si>
+  <si>
+    <t>2001401678</t>
+  </si>
+  <si>
+    <t>2001401677</t>
+  </si>
+  <si>
+    <t>200120275</t>
+  </si>
+  <si>
+    <t>200120279</t>
+  </si>
+  <si>
+    <t>Spot bonus</t>
+  </si>
+  <si>
+    <t>260.57</t>
+  </si>
+  <si>
+    <t>3,908.55</t>
+  </si>
+  <si>
+    <t>234.51</t>
+  </si>
+  <si>
+    <t>4143.06</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestSuite\branches\bau_environment\WppRegPack\MPLReports\Critical_Regression\Malaysia\2001\Print Job Quote-8.pdf</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestSuite\branches\bau_environment\WppRegPack\MPLReports\Critical_Regression\Malaysia\2001\Print Job Order Confirmation-2.pdf</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestSuite\branches\bau_environment\WppRegPack\MPLReports\Critical_Regression\Malaysia\2001\Print Invoice Editing-9.pdf</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestSuite\branches\bau_environment\WppRegPack\MPLReports\Critical_Regression\Malaysia\2001\Print Job Invoice-2.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001401679
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001401679
+</t>
+  </si>
+  <si>
+    <t>2001451073</t>
+  </si>
+  <si>
+    <t>200118904</t>
+  </si>
+  <si>
+    <t>2001401679</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -5155,7 +5292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5341,6 +5478,9 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5622,7 +5762,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -5705,13 +5845,13 @@
         <v>989</v>
       </c>
       <c r="C5" t="s">
-        <v>1453</v>
+        <v>1574</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -5719,7 +5859,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -5928,14 +6068,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6159,7 +6299,7 @@
         <v>990</v>
       </c>
       <c r="E4" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="F4" t="s">
         <v>510</v>
@@ -6175,14 +6315,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6231,7 +6371,7 @@
         <v>46</v>
       </c>
       <c r="E3" s="48">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -6248,7 +6388,7 @@
         <v>1108</v>
       </c>
       <c r="E4" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -6493,7 +6633,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -6529,7 +6669,7 @@
         <v>1144</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -6570,10 +6710,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -6595,7 +6735,7 @@
         <v>1145</v>
       </c>
       <c r="C8" s="90" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6705,7 +6845,7 @@
         <v>186</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6716,7 +6856,7 @@
         <v>1143</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -6747,8 +6887,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
-    <hyperlink ref="C8" r:id="rId2" display="2025_AutomationEmpy@gmail.com"/>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="C8" r:id="rId2" display="2025_AutomationEmpy@gmail.com" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -6756,7 +6896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -6799,7 +6939,7 @@
         <v>1281</v>
       </c>
       <c r="D2" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6839,7 +6979,7 @@
         <v>1069</v>
       </c>
       <c r="D5" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6861,13 +7001,13 @@
         <v>45</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6875,13 +7015,13 @@
         <v>46</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6905,7 +7045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -6929,7 +7069,7 @@
         <v>1063</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6940,7 +7080,7 @@
         <v>1144</v>
       </c>
       <c r="C2" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -6973,7 +7113,7 @@
         <v>1063</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -6995,7 +7135,7 @@
         <v>1338</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7017,7 +7157,7 @@
         <v>1144</v>
       </c>
       <c r="C9" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -7127,7 +7267,7 @@
         <v>186</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -7138,7 +7278,7 @@
         <v>1143</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -7182,7 +7322,7 @@
         <v>1338</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -7193,7 +7333,7 @@
         <v>1339</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -7204,13 +7344,13 @@
         <v>1146</v>
       </c>
       <c r="C26" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" display="1203_TestEmployeeAutomation@gmail.com"/>
-    <hyperlink ref="C9" r:id="rId2" display="1203_TestEmployeeAutomation@gmail.com"/>
+    <hyperlink ref="B9" r:id="rId1" display="1203_TestEmployeeAutomation@gmail.com" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="C9" r:id="rId2" display="1203_TestEmployeeAutomation@gmail.com" xr:uid="{00000000-0004-0000-0E00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -7218,7 +7358,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -7280,7 +7420,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -7346,7 +7486,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -7393,7 +7533,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -7704,46 +7844,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:FE95"/>
+  <dimension ref="A1:FF99"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71:B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" customWidth="true" style="19" width="39.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="19" width="27.85546875" collapsed="true"/>
-    <col min="9" max="161" customWidth="true" style="19" width="32.0" collapsed="true"/>
-    <col min="162" max="16384" style="19" width="9.140625" collapsed="true"/>
+    <col min="1" max="8" customWidth="true" style="19" width="39.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="19" width="27.85546875" collapsed="true"/>
+    <col min="10" max="162" customWidth="true" style="19" width="32.0" collapsed="true"/>
+    <col min="163" max="16384" style="19" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:161" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>175</v>
       </c>
       <c r="B1" s="10">
         <v>2001</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10">
+      <c r="C1" s="10">
         <v>2001</v>
       </c>
+      <c r="D1" s="10"/>
       <c r="E1" s="10">
+        <v>2001</v>
+      </c>
+      <c r="F1" s="10">
         <v>2011</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10">
         <v>2025</v>
       </c>
-      <c r="H1" s="10">
+      <c r="I1" s="10">
         <v>20234</v>
       </c>
-      <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -7896,454 +8038,509 @@
       <c r="FC1" s="10"/>
       <c r="FD1" s="10"/>
       <c r="FE1" s="10"/>
-    </row>
-    <row r="2" spans="1:161" x14ac:dyDescent="0.25">
+      <c r="FF1" s="10"/>
+    </row>
+    <row r="2" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>1466</v>
+        <v>1619</v>
       </c>
       <c r="C2" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="D2" t="s">
-        <v>1478</v>
+        <v>1465</v>
       </c>
       <c r="E2" t="s">
-        <v>1460</v>
+        <v>1477</v>
       </c>
       <c r="F2" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="G2" t="s">
+        <v>1459</v>
+      </c>
+      <c r="H2" t="s">
         <v>1409</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>1277</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>1107</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>1259</v>
       </c>
     </row>
-    <row r="3" spans="1:161" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="B3" t="s">
-        <v>1538</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>1478</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1524</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1464</v>
+      <c r="C3" t="s">
+        <v>1537</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>1477</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1523</v>
       </c>
       <c r="G3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="H3" t="s">
         <v>1340</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>1148</v>
       </c>
     </row>
-    <row r="4" spans="1:161" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>183</v>
       </c>
       <c r="B4" t="s">
-        <v>1563</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1520</v>
+        <v>1602</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1553</v>
       </c>
       <c r="E4" t="s">
-        <v>1473</v>
-      </c>
-      <c r="F4" s="48" t="s">
-        <v>1466</v>
-      </c>
-      <c r="G4" t="s">
+        <v>1519</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1472</v>
+      </c>
+      <c r="G4" s="48" t="s">
+        <v>1465</v>
+      </c>
+      <c r="H4" t="s">
         <v>1367</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>1150</v>
       </c>
     </row>
-    <row r="5" spans="1:161" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>199</v>
       </c>
       <c r="B5" t="s">
-        <v>1557</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1515</v>
+        <v>1605</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1547</v>
       </c>
       <c r="E5" t="s">
-        <v>1467</v>
-      </c>
-      <c r="F5">
+        <v>1514</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1466</v>
+      </c>
+      <c r="G5">
         <v>200120274</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>1360</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="I5" s="19" t="s">
         <v>1140</v>
       </c>
     </row>
-    <row r="6" spans="1:161" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>710</v>
       </c>
       <c r="B6" t="s">
-        <v>1560</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>1517</v>
+        <v>1606</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1550</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>1468</v>
-      </c>
-      <c r="G6" t="s">
+        <v>1516</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>1467</v>
+      </c>
+      <c r="H6" t="s">
         <v>1364</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>1157</v>
       </c>
     </row>
-    <row r="7" spans="1:161" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>711</v>
       </c>
       <c r="B7" t="s">
-        <v>1559</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>1516</v>
+        <v>1549</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1549</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>1469</v>
-      </c>
-      <c r="G7" t="s">
+        <v>1515</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H7" t="s">
         <v>1361</v>
-      </c>
-      <c r="H7" t="s">
-        <v>1152</v>
       </c>
       <c r="I7" t="s">
         <v>1152</v>
       </c>
-    </row>
-    <row r="8" spans="1:161" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>1020</v>
       </c>
       <c r="B8" t="s">
         <v>1432</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" t="s">
         <v>1432</v>
       </c>
       <c r="E8" t="s">
         <v>1432</v>
       </c>
-      <c r="G8" t="s">
-        <v>1141</v>
+      <c r="F8" t="s">
+        <v>1432</v>
       </c>
       <c r="H8" t="s">
         <v>1141</v>
       </c>
-    </row>
-    <row r="9" spans="1:161" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>1021</v>
       </c>
       <c r="B9" t="s">
         <v>1444</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" t="s">
         <v>1444</v>
       </c>
       <c r="E9" t="s">
         <v>1444</v>
       </c>
-      <c r="G9" t="s">
-        <v>995</v>
+      <c r="F9" t="s">
+        <v>1444</v>
       </c>
       <c r="H9" t="s">
         <v>995</v>
       </c>
-    </row>
-    <row r="10" spans="1:161" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>1022</v>
       </c>
       <c r="B10" t="s">
-        <v>1562</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>1519</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1471</v>
-      </c>
-      <c r="G10" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1552</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>1518</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1470</v>
+      </c>
+      <c r="H10" t="s">
         <v>1366</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>1142</v>
       </c>
     </row>
-    <row r="11" spans="1:161" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>1023</v>
       </c>
     </row>
-    <row r="12" spans="1:161" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>1024</v>
       </c>
     </row>
-    <row r="13" spans="1:161" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>970</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>1540</v>
-      </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="19" t="s">
-        <v>1494</v>
-      </c>
+        <v>1575</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D13" s="49"/>
       <c r="E13" s="19" t="s">
+        <v>1493</v>
+      </c>
+      <c r="F13" s="19" t="s">
         <v>1434</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>1346</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>1316</v>
       </c>
     </row>
-    <row r="14" spans="1:161" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>1025</v>
       </c>
-      <c r="B14" s="19" t="s">
-        <v>1539</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>1495</v>
+      <c r="B14" s="49" t="s">
+        <v>1576</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>1538</v>
       </c>
       <c r="E14" s="19" t="s">
+        <v>1494</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>1433</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>1347</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>1317</v>
       </c>
     </row>
-    <row r="15" spans="1:161" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>971</v>
       </c>
       <c r="B15" s="49" t="s">
-        <v>1541</v>
-      </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="19" t="s">
-        <v>1502</v>
-      </c>
+        <v>1577</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D15" s="49"/>
       <c r="E15" s="19" t="s">
+        <v>1501</v>
+      </c>
+      <c r="F15" s="19" t="s">
         <v>1435</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>1348</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>1318</v>
       </c>
     </row>
-    <row r="16" spans="1:161" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>1026</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>1543</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>1503</v>
+      <c r="B16" s="49" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>1542</v>
       </c>
       <c r="E16" s="19" t="s">
+        <v>1502</v>
+      </c>
+      <c r="F16" s="19" t="s">
         <v>1436</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>1349</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>1319</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>972</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>1542</v>
-      </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="19" t="s">
-        <v>1504</v>
-      </c>
+        <v>1580</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>1541</v>
+      </c>
+      <c r="D17" s="49"/>
       <c r="E17" s="19" t="s">
+        <v>1503</v>
+      </c>
+      <c r="F17" s="19" t="s">
         <v>1437</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>1350</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>1320</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>1027</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>1544</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>1505</v>
+      <c r="B18" s="49" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>1543</v>
       </c>
       <c r="E18" s="19" t="s">
+        <v>1504</v>
+      </c>
+      <c r="F18" s="19" t="s">
         <v>1438</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>1351</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>1321</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>1028</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>1029</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>187</v>
       </c>
       <c r="B21" t="s">
-        <v>1545</v>
-      </c>
-      <c r="C21"/>
-      <c r="D21" t="s">
-        <v>1506</v>
-      </c>
+        <v>1582</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1544</v>
+      </c>
+      <c r="D21"/>
       <c r="E21" t="s">
+        <v>1505</v>
+      </c>
+      <c r="F21" t="s">
         <v>1439</v>
       </c>
-      <c r="F21"/>
-      <c r="G21" t="s">
+      <c r="G21"/>
+      <c r="H21" t="s">
         <v>1352</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>1322</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>1030</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>1031</v>
       </c>
       <c r="B23" t="s">
-        <v>1578</v>
-      </c>
-      <c r="D23" t="s">
-        <v>1534</v>
+        <v>1592</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1568</v>
       </c>
       <c r="E23" t="s">
-        <v>1484</v>
-      </c>
-      <c r="G23" t="s">
+        <v>1533</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H23" t="s">
         <v>1395</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>1229</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>1149</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>1032</v>
       </c>
       <c r="B25" t="s">
-        <v>1478</v>
-      </c>
-      <c r="C25"/>
-      <c r="D25" t="s">
-        <v>1478</v>
-      </c>
+        <v>1619</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D25"/>
       <c r="E25" t="s">
-        <v>1478</v>
-      </c>
-      <c r="F25"/>
-      <c r="G25" t="s">
+        <v>1477</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1477</v>
+      </c>
+      <c r="G25"/>
+      <c r="H25" t="s">
         <v>1409</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>1277</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>1033</v>
       </c>
       <c r="B26" t="s">
         <v>201</v>
       </c>
-      <c r="C26"/>
-      <c r="D26" t="s">
+      <c r="C26" t="s">
         <v>201</v>
       </c>
+      <c r="D26"/>
       <c r="E26" t="s">
         <v>201</v>
       </c>
-      <c r="F26"/>
-      <c r="G26" t="s">
+      <c r="F26" t="s">
         <v>201</v>
       </c>
+      <c r="G26"/>
       <c r="H26" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1034</v>
       </c>
@@ -8353,52 +8550,59 @@
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1035</v>
       </c>
       <c r="B28" t="s">
-        <v>1561</v>
-      </c>
-      <c r="C28"/>
-      <c r="D28" s="48" t="s">
-        <v>1518</v>
-      </c>
+        <v>1607</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1551</v>
+      </c>
+      <c r="D28"/>
       <c r="E28" s="48" t="s">
-        <v>1470</v>
-      </c>
-      <c r="F28"/>
-      <c r="G28" t="s">
+        <v>1517</v>
+      </c>
+      <c r="F28" s="48" t="s">
+        <v>1469</v>
+      </c>
+      <c r="G28"/>
+      <c r="H28" t="s">
         <v>1365</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>1158</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1036</v>
       </c>
       <c r="B29" t="s">
         <v>1427</v>
       </c>
-      <c r="C29"/>
-      <c r="D29" t="s">
+      <c r="C29" t="s">
         <v>1427</v>
       </c>
+      <c r="D29"/>
       <c r="E29" t="s">
         <v>1427</v>
       </c>
-      <c r="F29"/>
-      <c r="G29" t="s">
+      <c r="F29" t="s">
+        <v>1427</v>
+      </c>
+      <c r="G29"/>
+      <c r="H29" t="s">
         <v>1404</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>958</v>
       </c>
@@ -8408,8 +8612,9 @@
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1037</v>
       </c>
@@ -8419,8 +8624,9 @@
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H31"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1038</v>
       </c>
@@ -8430,8 +8636,9 @@
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H32"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1039</v>
       </c>
@@ -8441,8 +8648,9 @@
       <c r="E33"/>
       <c r="F33"/>
       <c r="G33"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H33"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1040</v>
       </c>
@@ -8452,8 +8660,9 @@
       <c r="E34"/>
       <c r="F34"/>
       <c r="G34"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H34"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1041</v>
       </c>
@@ -8463,8 +8672,9 @@
       <c r="E35"/>
       <c r="F35"/>
       <c r="G35"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H35"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1042</v>
       </c>
@@ -8474,8 +8684,9 @@
       <c r="E36"/>
       <c r="F36"/>
       <c r="G36"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H36"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1043</v>
       </c>
@@ -8485,8 +8696,9 @@
       <c r="E37"/>
       <c r="F37"/>
       <c r="G37"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H37"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1044</v>
       </c>
@@ -8496,8 +8708,9 @@
       <c r="E38"/>
       <c r="F38"/>
       <c r="G38"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H38"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1045</v>
       </c>
@@ -8507,8 +8720,9 @@
       <c r="E39"/>
       <c r="F39"/>
       <c r="G39"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H39"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1046</v>
       </c>
@@ -8518,59 +8732,63 @@
       <c r="E40"/>
       <c r="F40"/>
       <c r="G40"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H40"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>1047</v>
       </c>
-      <c r="G41" s="19" t="s">
+      <c r="H41" s="19" t="s">
         <v>1354</v>
       </c>
-      <c r="H41" s="19" t="s">
+      <c r="I41" s="19" t="s">
         <v>1277</v>
-      </c>
-      <c r="I41" t="s">
-        <v>1107</v>
       </c>
       <c r="J41" t="s">
         <v>1107</v>
       </c>
       <c r="K41" t="s">
+        <v>1107</v>
+      </c>
+      <c r="L41" t="s">
         <v>1263</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>1197</v>
       </c>
-      <c r="G42" s="19" t="s">
+      <c r="H42" s="19" t="s">
         <v>1392</v>
       </c>
-      <c r="H42" s="19" t="s">
+      <c r="I42" s="19" t="s">
         <v>1279</v>
       </c>
-      <c r="I42" s="19" t="s">
+      <c r="J42" s="19" t="s">
         <v>1198</v>
       </c>
-      <c r="J42" s="19" t="s">
+      <c r="K42" s="19" t="s">
         <v>1255</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>1259</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1048</v>
       </c>
-      <c r="B43"/>
+      <c r="B43" t="s">
+        <v>1630</v>
+      </c>
       <c r="C43"/>
       <c r="D43"/>
       <c r="E43"/>
       <c r="F43"/>
       <c r="G43"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H43"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1049</v>
       </c>
@@ -8580,38 +8798,39 @@
       <c r="E44"/>
       <c r="F44"/>
       <c r="G44"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H44"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>1050</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>1051</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>1052</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>1054</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>1055</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1056</v>
       </c>
@@ -8621,8 +8840,9 @@
       <c r="E51"/>
       <c r="F51"/>
       <c r="G51"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H51"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1057</v>
       </c>
@@ -8632,8 +8852,9 @@
       <c r="E52"/>
       <c r="F52"/>
       <c r="G52"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H52"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1058</v>
       </c>
@@ -8643,8 +8864,9 @@
       <c r="E53"/>
       <c r="F53"/>
       <c r="G53"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H53"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1059</v>
       </c>
@@ -8654,8 +8876,9 @@
       <c r="E54"/>
       <c r="F54"/>
       <c r="G54"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H54"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1060</v>
       </c>
@@ -8665,8 +8888,9 @@
       <c r="E55"/>
       <c r="F55"/>
       <c r="G55"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H55"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1061</v>
       </c>
@@ -8676,8 +8900,9 @@
       <c r="E56"/>
       <c r="F56"/>
       <c r="G56"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H56"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1062</v>
       </c>
@@ -8687,656 +8912,767 @@
       <c r="E57"/>
       <c r="F57"/>
       <c r="G57"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H57"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>248</v>
       </c>
       <c r="B58" t="s">
-        <v>1481</v>
-      </c>
-      <c r="C58"/>
-      <c r="D58" t="s">
-        <v>1481</v>
-      </c>
+        <v>1480</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1480</v>
+      </c>
+      <c r="D58"/>
       <c r="E58" t="s">
-        <v>1481</v>
-      </c>
-      <c r="F58"/>
-      <c r="G58" t="s">
+        <v>1480</v>
+      </c>
+      <c r="F58" t="s">
+        <v>1480</v>
+      </c>
+      <c r="G58"/>
+      <c r="H58" t="s">
         <v>1403</v>
       </c>
-      <c r="H58" t="s">
+      <c r="I58" t="s">
         <v>1151</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>1072</v>
       </c>
       <c r="B59" t="s">
         <v>286</v>
       </c>
-      <c r="C59"/>
-      <c r="D59" t="s">
+      <c r="C59" t="s">
         <v>286</v>
       </c>
+      <c r="D59"/>
       <c r="E59" t="s">
         <v>286</v>
       </c>
-      <c r="F59"/>
-      <c r="G59" t="s">
+      <c r="F59" t="s">
         <v>286</v>
       </c>
+      <c r="G59"/>
       <c r="H59" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>1131</v>
       </c>
       <c r="B60" t="s">
+        <v>1625</v>
+      </c>
+      <c r="C60" t="s">
         <v>1278</v>
       </c>
-      <c r="C60"/>
-      <c r="D60" t="s">
-        <v>1530</v>
-      </c>
+      <c r="D60"/>
       <c r="E60" t="s">
+        <v>1529</v>
+      </c>
+      <c r="F60" t="s">
         <v>1278</v>
       </c>
-      <c r="F60"/>
-      <c r="G60" t="s">
+      <c r="G60"/>
+      <c r="H60" t="s">
         <v>1410</v>
       </c>
-      <c r="H60" t="s">
+      <c r="I60" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>1132</v>
       </c>
       <c r="B61" t="s">
-        <v>1556</v>
-      </c>
-      <c r="C61"/>
-      <c r="D61" t="s">
-        <v>1531</v>
-      </c>
+        <v>1626</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1546</v>
+      </c>
+      <c r="D61"/>
       <c r="E61" t="s">
+        <v>1530</v>
+      </c>
+      <c r="F61" t="s">
         <v>1278</v>
       </c>
-      <c r="F61"/>
-      <c r="G61" t="s">
+      <c r="G61"/>
+      <c r="H61" t="s">
         <v>1411</v>
       </c>
-      <c r="H61" t="s">
+      <c r="I61" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1153</v>
       </c>
       <c r="B62" t="s">
         <v>1284</v>
       </c>
-      <c r="C62"/>
-      <c r="D62" t="s">
+      <c r="C62" t="s">
         <v>1284</v>
       </c>
+      <c r="D62"/>
       <c r="E62" t="s">
         <v>1284</v>
       </c>
-      <c r="F62"/>
-      <c r="G62" t="s">
+      <c r="F62" t="s">
         <v>1284</v>
       </c>
+      <c r="G62"/>
       <c r="H62" t="s">
         <v>1284</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>1154</v>
       </c>
       <c r="B63" t="s">
         <v>1155</v>
       </c>
-      <c r="C63"/>
-      <c r="D63" s="96" t="s">
+      <c r="C63" t="s">
         <v>1155</v>
       </c>
+      <c r="D63"/>
       <c r="E63" s="96" t="s">
         <v>1155</v>
       </c>
-      <c r="F63"/>
-      <c r="G63" t="s">
+      <c r="F63" s="96" t="s">
+        <v>1155</v>
+      </c>
+      <c r="G63"/>
+      <c r="H63" t="s">
         <v>1363</v>
       </c>
-      <c r="H63" t="s">
+      <c r="I63" t="s">
         <v>1155</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>1156</v>
       </c>
       <c r="B64" t="s">
         <v>1155</v>
       </c>
-      <c r="C64"/>
-      <c r="D64" s="96" t="s">
+      <c r="C64" t="s">
         <v>1155</v>
       </c>
+      <c r="D64"/>
       <c r="E64" s="96" t="s">
         <v>1155</v>
       </c>
-      <c r="F64"/>
-      <c r="G64" t="s">
+      <c r="F64" s="96" t="s">
+        <v>1155</v>
+      </c>
+      <c r="G64"/>
+      <c r="H64" t="s">
         <v>1363</v>
       </c>
-      <c r="H64" t="s">
+      <c r="I64" t="s">
         <v>1155</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1159</v>
       </c>
       <c r="B65" t="s">
-        <v>1560</v>
-      </c>
-      <c r="C65"/>
-      <c r="D65" t="s">
-        <v>1517</v>
-      </c>
+        <v>1606</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D65"/>
       <c r="E65" t="s">
-        <v>1468</v>
-      </c>
-      <c r="F65"/>
-      <c r="G65" t="s">
+        <v>1516</v>
+      </c>
+      <c r="F65" t="s">
+        <v>1467</v>
+      </c>
+      <c r="G65"/>
+      <c r="H65" t="s">
         <v>1364</v>
       </c>
-      <c r="H65" t="s">
+      <c r="I65" t="s">
         <v>1157</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1196</v>
       </c>
-      <c r="B66"/>
+      <c r="B66" t="s">
+        <v>1627</v>
+      </c>
       <c r="C66"/>
       <c r="D66"/>
       <c r="E66"/>
       <c r="F66"/>
-      <c r="G66" t="s">
+      <c r="G66"/>
+      <c r="H66" t="s">
         <v>1391</v>
       </c>
-      <c r="H66" t="s">
+      <c r="I66" t="s">
         <v>1260</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1199</v>
       </c>
       <c r="B67" t="s">
-        <v>1571</v>
-      </c>
-      <c r="C67"/>
-      <c r="D67" t="s">
-        <v>1526</v>
-      </c>
+        <v>1615</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1561</v>
+      </c>
+      <c r="D67"/>
       <c r="E67" t="s">
-        <v>1476</v>
-      </c>
-      <c r="F67"/>
-      <c r="G67" t="s">
+        <v>1525</v>
+      </c>
+      <c r="F67" t="s">
+        <v>1475</v>
+      </c>
+      <c r="G67"/>
+      <c r="H67" t="s">
         <v>1393</v>
       </c>
-      <c r="H67" t="s">
+      <c r="I67" t="s">
         <v>1257</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1200</v>
       </c>
       <c r="B68" t="s">
-        <v>1564</v>
-      </c>
-      <c r="C68"/>
-      <c r="D68" t="s">
-        <v>1525</v>
-      </c>
+        <v>1616</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1554</v>
+      </c>
+      <c r="D68"/>
       <c r="E68" t="s">
-        <v>1474</v>
-      </c>
-      <c r="F68"/>
-      <c r="G68" t="s">
+        <v>1524</v>
+      </c>
+      <c r="F68" t="s">
+        <v>1473</v>
+      </c>
+      <c r="G68"/>
+      <c r="H68" t="s">
         <v>1392</v>
       </c>
-      <c r="H68" t="s">
+      <c r="I68" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1201</v>
       </c>
       <c r="B69" t="s">
-        <v>1466</v>
-      </c>
-      <c r="C69"/>
-      <c r="D69" t="s">
-        <v>1460</v>
-      </c>
+        <v>1596</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D69"/>
       <c r="E69" t="s">
-        <v>1460</v>
-      </c>
-      <c r="F69"/>
-      <c r="G69" t="s">
+        <v>1459</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1459</v>
+      </c>
+      <c r="G69"/>
+      <c r="H69" t="s">
         <v>1354</v>
       </c>
-      <c r="H69" t="s">
+      <c r="I69" t="s">
         <v>1259</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>1246</v>
       </c>
       <c r="B70" t="s">
         <v>1288</v>
       </c>
-      <c r="C70"/>
-      <c r="D70" t="s">
+      <c r="C70" t="s">
         <v>1288</v>
       </c>
+      <c r="D70"/>
       <c r="E70" t="s">
         <v>1288</v>
       </c>
-      <c r="F70"/>
-      <c r="G70" t="s">
+      <c r="F70" t="s">
         <v>1288</v>
       </c>
+      <c r="G70"/>
       <c r="H70" t="s">
         <v>1288</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1247</v>
       </c>
-      <c r="B71" s="48" t="s">
-        <v>1564</v>
-      </c>
-      <c r="C71"/>
-      <c r="D71" t="s">
-        <v>1527</v>
-      </c>
-      <c r="E71"/>
+      <c r="B71" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C71" s="48" t="s">
+        <v>1554</v>
+      </c>
+      <c r="D71"/>
+      <c r="E71" t="s">
+        <v>1526</v>
+      </c>
       <c r="F71"/>
-      <c r="G71" t="s">
+      <c r="G71"/>
+      <c r="H71" t="s">
         <v>1412</v>
       </c>
-      <c r="H71" t="s">
+      <c r="I71" t="s">
         <v>1248</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1249</v>
       </c>
       <c r="B72" t="s">
-        <v>1466</v>
-      </c>
-      <c r="C72"/>
-      <c r="D72" t="s">
-        <v>1466</v>
-      </c>
-      <c r="E72"/>
+        <v>1619</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D72"/>
+      <c r="E72" t="s">
+        <v>1465</v>
+      </c>
       <c r="F72"/>
-      <c r="G72" t="s">
+      <c r="G72"/>
+      <c r="H72" t="s">
         <v>1409</v>
       </c>
-      <c r="H72" t="s">
+      <c r="I72" t="s">
         <v>1107</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>1253</v>
       </c>
       <c r="B73" t="s">
-        <v>1566</v>
-      </c>
-      <c r="C73"/>
-      <c r="D73" t="s">
-        <v>1528</v>
-      </c>
+        <v>1633</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1556</v>
+      </c>
+      <c r="D73"/>
       <c r="E73" t="s">
-        <v>1479</v>
-      </c>
-      <c r="F73"/>
-      <c r="G73" t="s">
+        <v>1527</v>
+      </c>
+      <c r="F73" t="s">
+        <v>1478</v>
+      </c>
+      <c r="G73"/>
+      <c r="H73" t="s">
         <v>1413</v>
       </c>
-      <c r="H73" t="s">
+      <c r="I73" t="s">
         <v>1279</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1254</v>
       </c>
       <c r="B74" t="s">
-        <v>1464</v>
-      </c>
-      <c r="C74"/>
-      <c r="D74" t="s">
-        <v>1466</v>
-      </c>
+        <v>1619</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D74"/>
       <c r="E74" t="s">
-        <v>1478</v>
-      </c>
-      <c r="F74"/>
-      <c r="G74" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F74" t="s">
+        <v>1477</v>
+      </c>
+      <c r="G74"/>
+      <c r="H74" t="s">
         <v>1409</v>
       </c>
-      <c r="H74" t="s">
+      <c r="I74" t="s">
         <v>1277</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>1256</v>
       </c>
       <c r="B75" t="s">
-        <v>1577</v>
-      </c>
-      <c r="C75"/>
-      <c r="D75" t="s">
-        <v>1529</v>
-      </c>
+        <v>1632</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1567</v>
+      </c>
+      <c r="D75"/>
       <c r="E75" t="s">
-        <v>1480</v>
-      </c>
-      <c r="F75"/>
-      <c r="G75" t="s">
+        <v>1528</v>
+      </c>
+      <c r="F75" t="s">
+        <v>1479</v>
+      </c>
+      <c r="G75"/>
+      <c r="H75" t="s">
         <v>1414</v>
       </c>
-      <c r="H75" t="s">
+      <c r="I75" t="s">
         <v>1280</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>1261</v>
       </c>
-      <c r="B76"/>
+      <c r="B76" t="s">
+        <v>1628</v>
+      </c>
       <c r="C76"/>
       <c r="D76"/>
       <c r="E76"/>
       <c r="F76"/>
       <c r="G76"/>
-      <c r="H76" t="s">
+      <c r="H76"/>
+      <c r="I76" t="s">
         <v>1262</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
         <v>1264</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>1265</v>
       </c>
-      <c r="H78"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
         <v>1266</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
         <v>1267</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="19" t="s">
         <v>1268</v>
       </c>
-      <c r="I81" t="s">
+      <c r="J81" t="s">
         <v>1107</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">
         <v>1269</v>
       </c>
-      <c r="I82" t="s">
+      <c r="J82" t="s">
         <v>1248</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1273</v>
       </c>
       <c r="B83" t="s">
-        <v>1565</v>
-      </c>
-      <c r="C83"/>
-      <c r="D83" t="s">
-        <v>1532</v>
-      </c>
+        <v>1617</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1555</v>
+      </c>
+      <c r="D83"/>
       <c r="E83" t="s">
-        <v>1475</v>
-      </c>
-      <c r="F83"/>
-      <c r="G83" t="s">
+        <v>1531</v>
+      </c>
+      <c r="F83" t="s">
+        <v>1474</v>
+      </c>
+      <c r="G83"/>
+      <c r="H83" t="s">
         <v>1408</v>
       </c>
-      <c r="H83" t="s">
+      <c r="I83" t="s">
         <v>1255</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1274</v>
       </c>
       <c r="B84" t="s">
-        <v>1460</v>
-      </c>
-      <c r="C84"/>
-      <c r="D84" t="s">
-        <v>1478</v>
-      </c>
+        <v>1618</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D84"/>
       <c r="E84" t="s">
-        <v>1464</v>
-      </c>
-      <c r="F84"/>
-      <c r="G84" t="s">
+        <v>1477</v>
+      </c>
+      <c r="F84" t="s">
+        <v>1463</v>
+      </c>
+      <c r="G84"/>
+      <c r="H84" t="s">
         <v>1406</v>
       </c>
-      <c r="H84" t="s">
+      <c r="I84" t="s">
         <v>1107</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1275</v>
       </c>
-      <c r="B85" t="s">
-        <v>1574</v>
-      </c>
-      <c r="C85"/>
-      <c r="D85" t="s">
-        <v>1533</v>
-      </c>
+      <c r="B85"/>
+      <c r="C85" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D85"/>
       <c r="E85" t="s">
-        <v>1477</v>
-      </c>
-      <c r="F85"/>
-      <c r="G85" t="s">
+        <v>1532</v>
+      </c>
+      <c r="F85" t="s">
+        <v>1476</v>
+      </c>
+      <c r="G85"/>
+      <c r="H85" t="s">
         <v>1407</v>
       </c>
-      <c r="H85" t="s">
+      <c r="I85" t="s">
         <v>1276</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1285</v>
       </c>
       <c r="B86" t="s">
-        <v>1521</v>
-      </c>
-      <c r="C86"/>
-      <c r="D86" t="s">
-        <v>1521</v>
-      </c>
+        <v>1608</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1520</v>
+      </c>
+      <c r="D86"/>
       <c r="E86" t="s">
+        <v>1520</v>
+      </c>
+      <c r="F86" t="s">
         <v>1278</v>
       </c>
-      <c r="F86"/>
-      <c r="G86" t="s">
+      <c r="G86"/>
+      <c r="H86" t="s">
         <v>1399</v>
       </c>
-      <c r="H86" t="s">
+      <c r="I86" t="s">
         <v>1287</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1289</v>
       </c>
-      <c r="B87" t="s">
-        <v>1584</v>
-      </c>
-      <c r="C87"/>
-      <c r="D87" t="s">
-        <v>1522</v>
-      </c>
+      <c r="B87"/>
+      <c r="C87" t="s">
+        <v>1570</v>
+      </c>
+      <c r="D87"/>
       <c r="E87" t="s">
-        <v>1485</v>
-      </c>
-      <c r="F87"/>
-      <c r="G87" t="s">
+        <v>1521</v>
+      </c>
+      <c r="F87" t="s">
+        <v>1484</v>
+      </c>
+      <c r="G87"/>
+      <c r="H87" t="s">
         <v>1400</v>
       </c>
-      <c r="H87" t="s">
+      <c r="I87" t="s">
         <v>1290</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1291</v>
       </c>
-      <c r="B88" t="s">
-        <v>1523</v>
-      </c>
-      <c r="C88"/>
-      <c r="D88" t="s">
-        <v>1523</v>
-      </c>
+      <c r="B88"/>
+      <c r="C88" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D88"/>
       <c r="E88" t="s">
+        <v>1522</v>
+      </c>
+      <c r="F88" t="s">
         <v>1278</v>
       </c>
-      <c r="F88"/>
-      <c r="G88" t="s">
+      <c r="G88"/>
+      <c r="H88" t="s">
         <v>1401</v>
       </c>
-      <c r="H88" t="s">
+      <c r="I88" t="s">
         <v>1292</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1323</v>
       </c>
       <c r="B89" t="s">
         <v>510</v>
       </c>
-      <c r="C89"/>
-      <c r="D89" t="s">
+      <c r="C89" t="s">
         <v>510</v>
       </c>
+      <c r="D89"/>
       <c r="E89" t="s">
         <v>510</v>
       </c>
-      <c r="F89"/>
-      <c r="G89" t="s">
+      <c r="F89" t="s">
         <v>510</v>
       </c>
+      <c r="G89"/>
       <c r="H89" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I89" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
         <v>1334</v>
       </c>
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>1341</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B91"/>
+      <c r="C91" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D91"/>
+      <c r="E91" t="s">
         <v>1507</v>
       </c>
-      <c r="B91" t="s">
-        <v>1546</v>
-      </c>
-      <c r="C91"/>
-      <c r="D91" t="s">
-        <v>1508</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>1567</v>
+        <v>1557</v>
       </c>
       <c r="B92" t="s">
-        <v>1568</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1614</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>1569</v>
+        <v>1559</v>
       </c>
       <c r="B93" t="s">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1560</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>1562</v>
+      </c>
+      <c r="B94"/>
+      <c r="C94" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1631</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>1572</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B96" t="s">
+        <v>1609</v>
+      </c>
+      <c r="C96" t="s">
         <v>1573</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>1575</v>
-      </c>
-      <c r="B95" t="s">
-        <v>1576</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s">
-        <v>1588</v>
-      </c>
-      <c r="B96" t="s">
-        <v>1589</v>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1604</v>
       </c>
     </row>
   </sheetData>
@@ -9346,7 +9682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -9408,7 +9744,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="D5" t="s">
         <v>201</v>
@@ -9421,7 +9757,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -9464,7 +9800,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -9519,7 +9855,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -9555,7 +9891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -9618,7 +9954,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -9669,7 +10005,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -9896,7 +10232,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -10118,7 +10454,7 @@
         <v>2001</v>
       </c>
       <c r="D6" s="91" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
   </sheetData>
@@ -10128,7 +10464,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -10189,7 +10525,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -10246,7 +10582,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -11428,7 +11764,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -11526,7 +11862,7 @@
         <v>1402</v>
       </c>
       <c r="D6" s="92" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -11564,7 +11900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -11667,7 +12003,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -11772,7 +12108,7 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -11843,7 +12179,7 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -11931,7 +12267,7 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -12071,16 +12407,16 @@
         <v>2001</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="E6" t="s">
-        <v>1559</v>
+        <v>1549</v>
       </c>
       <c r="F6" t="s">
-        <v>1558</v>
+        <v>1548</v>
       </c>
     </row>
   </sheetData>
@@ -12090,7 +12426,7 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -12143,7 +12479,7 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -12181,7 +12517,7 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -12248,14 +12584,14 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12263,7 +12599,9 @@
     <col min="1" max="1" bestFit="true" customWidth="true" style="19" width="11.7109375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="19" width="24.42578125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="19" width="7.0" collapsed="true"/>
-    <col min="4" max="16384" style="19" width="9.140625" collapsed="true"/>
+    <col min="4" max="5" style="19" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="19" width="14.42578125" collapsed="true"/>
+    <col min="7" max="16384" style="19" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -12283,15 +12621,15 @@
         <v>1063</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="F2" t="s">
-        <v>1466</v>
+      <c r="F2">
+        <v>200120277</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -12311,7 +12649,7 @@
         <v>1270</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>1270</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -12343,8 +12681,8 @@
       <c r="A6" s="19" t="s">
         <v>1251</v>
       </c>
-      <c r="F6" s="48" t="s">
-        <v>1564</v>
+      <c r="F6" s="98">
+        <v>2001401678</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -12360,7 +12698,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -14414,7 +14752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -14430,8 +14768,10 @@
     <col min="2" max="2" bestFit="true" customWidth="true" style="19" width="24.42578125" collapsed="true"/>
     <col min="3" max="4" style="19" width="9.140625" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="19" width="11.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="19" width="10.0" collapsed="true"/>
-    <col min="7" max="16384" style="19" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="19" width="16.5703125" collapsed="true"/>
+    <col min="7" max="10" style="19" width="9.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="19" width="12.140625" collapsed="true"/>
+    <col min="12" max="16384" style="19" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -14451,7 +14791,7 @@
         <v>1063</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -14462,7 +14802,7 @@
         <v>202522371</v>
       </c>
       <c r="F2">
-        <v>200120271</v>
+        <v>200120275</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -14510,15 +14850,15 @@
         <v>510</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>1251</v>
       </c>
       <c r="E6">
         <v>2025401646</v>
       </c>
-      <c r="F6" s="48" t="s">
-        <v>1565</v>
+      <c r="F6" s="98">
+        <v>2001401677</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -14536,7 +14876,7 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -14567,7 +14907,7 @@
         <v>1063</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -14592,14 +14932,14 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="A7:C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14617,7 +14957,7 @@
         <v>1063</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -14627,9 +14967,7 @@
       <c r="B2" s="19" t="s">
         <v>1409</v>
       </c>
-      <c r="C2" s="48" t="s">
-        <v>1464</v>
-      </c>
+      <c r="C2" s="48"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
@@ -14665,9 +15003,7 @@
       <c r="B6" s="19" t="s">
         <v>1413</v>
       </c>
-      <c r="C6" s="48" t="s">
-        <v>1566</v>
-      </c>
+      <c r="C6" s="48"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
@@ -14692,7 +15028,7 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -14789,7 +15125,7 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -14869,7 +15205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -14940,7 +15276,7 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -15126,7 +15462,7 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15177,7 +15513,7 @@
         <v>1394</v>
       </c>
       <c r="C5" s="84" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -15219,7 +15555,7 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15256,7 +15592,7 @@
         <v>1394</v>
       </c>
       <c r="C3" s="84" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -15299,7 +15635,7 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15354,7 +15690,7 @@
         <v>1394</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -15393,7 +15729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -15631,7 +15967,7 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -15766,7 +16102,7 @@
         <v>916</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="C9" s="48" t="s">
         <v>1342</v>
@@ -15780,7 +16116,7 @@
         <v>918</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="C10" s="48" t="s">
         <v>1343</v>
@@ -15998,10 +16334,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="B29" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -16009,20 +16345,20 @@
         <v>1206</v>
       </c>
       <c r="B30" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="B31" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="B32" t="s">
         <v>509</v>
@@ -16035,11 +16371,11 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16226,51 +16562,51 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1089</v>
+        <v>1581</v>
       </c>
       <c r="B17" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="C17" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="B18" t="s">
-        <v>1086</v>
+        <v>1090</v>
       </c>
       <c r="C18" t="s">
-        <v>1086</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1092</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>1093</v>
-      </c>
-      <c r="C19" s="48" t="s">
-        <v>1093</v>
+        <v>1091</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1086</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1094</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1086</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1086</v>
+        <v>1092</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>1093</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B21" t="s">
         <v>1086</v>
@@ -16281,85 +16617,96 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>204</v>
+        <v>1095</v>
       </c>
       <c r="B22" t="s">
-        <v>915</v>
+        <v>1086</v>
       </c>
       <c r="C22" t="s">
-        <v>915</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1096</v>
+        <v>204</v>
       </c>
       <c r="B23" t="s">
-        <v>931</v>
+        <v>915</v>
       </c>
       <c r="C23" t="s">
-        <v>931</v>
+        <v>915</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B24" t="s">
-        <v>1086</v>
+        <v>931</v>
       </c>
       <c r="C24" t="s">
-        <v>1086</v>
+        <v>931</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B25" t="s">
-        <v>1099</v>
+        <v>1086</v>
       </c>
       <c r="C25" t="s">
-        <v>1099</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="B26" t="s">
-        <v>1284</v>
+        <v>1099</v>
       </c>
       <c r="C26" t="s">
-        <v>1284</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1101</v>
-      </c>
-      <c r="B27">
-        <v>3000</v>
-      </c>
-      <c r="C27">
-        <v>3000</v>
+        <v>1100</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1284</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B28">
+        <v>3000</v>
+      </c>
+      <c r="C28">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>1102</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>300000</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>300000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-3200-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-3200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -16367,7 +16714,7 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -16441,7 +16788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -16527,7 +16874,7 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -16571,7 +16918,7 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -16628,7 +16975,7 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
@@ -16796,7 +17143,7 @@
         <v>266</v>
       </c>
       <c r="G4" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="H4" s="48" t="s">
         <v>961</v>
@@ -16809,7 +17156,7 @@
         <v>266</v>
       </c>
       <c r="M4" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="N4" s="48" t="s">
         <v>962</v>
@@ -16825,7 +17172,7 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17046,37 +17393,37 @@
     <row r="4" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="B5" t="s">
-        <v>1578</v>
+        <v>1592</v>
       </c>
       <c r="C5" t="s">
-        <v>1579</v>
+        <v>1569</v>
       </c>
       <c r="D5" t="s">
         <v>1013</v>
       </c>
       <c r="E5" t="s">
-        <v>1580</v>
+        <v>1593</v>
       </c>
       <c r="F5" t="s">
-        <v>1581</v>
+        <v>1594</v>
       </c>
       <c r="G5" t="s">
-        <v>1582</v>
+        <v>712</v>
       </c>
       <c r="H5" t="s">
-        <v>1583</v>
+        <v>1595</v>
       </c>
       <c r="I5" t="s">
-        <v>1580</v>
+        <v>1593</v>
       </c>
       <c r="J5" t="s">
         <v>266</v>
       </c>
       <c r="K5" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="L5" t="s">
         <v>1231</v>
@@ -17100,16 +17447,16 @@
         <v>1234</v>
       </c>
       <c r="S5" t="s">
-        <v>1583</v>
+        <v>1595</v>
       </c>
       <c r="T5" t="s">
-        <v>1580</v>
+        <v>1593</v>
       </c>
       <c r="U5" t="s">
         <v>266</v>
       </c>
       <c r="V5" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="W5" t="s">
         <v>1235</v>
@@ -17140,7 +17487,7 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17174,7 +17521,7 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -17220,14 +17567,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:AP5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17505,13 +17852,13 @@
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>201</v>
+        <v>2001</v>
       </c>
       <c r="C4" t="s">
+        <v>1453</v>
+      </c>
+      <c r="D4" t="s">
         <v>1454</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1455</v>
       </c>
       <c r="E4">
         <v>6</v>
@@ -17520,10 +17867,10 @@
         <v>1000</v>
       </c>
       <c r="G4" t="s">
+        <v>1455</v>
+      </c>
+      <c r="H4" t="s">
         <v>1456</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1457</v>
       </c>
       <c r="I4">
         <v>25</v>
@@ -17532,10 +17879,10 @@
         <v>500</v>
       </c>
       <c r="K4" t="s">
+        <v>1457</v>
+      </c>
+      <c r="L4" t="s">
         <v>1458</v>
-      </c>
-      <c r="L4" t="s">
-        <v>1459</v>
       </c>
       <c r="M4">
         <v>15</v>
@@ -17546,13 +17893,13 @@
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2001</v>
+        <v>201</v>
       </c>
       <c r="C5" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="D5" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="E5">
         <v>6</v>
@@ -17561,10 +17908,10 @@
         <v>1000</v>
       </c>
       <c r="G5" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="H5" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="I5">
         <v>25</v>
@@ -17573,10 +17920,10 @@
         <v>500</v>
       </c>
       <c r="K5" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="L5" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="M5">
         <v>10</v>
@@ -17592,7 +17939,7 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17685,7 +18032,7 @@
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17815,7 +18162,7 @@
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17912,7 +18259,7 @@
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17948,7 +18295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
   <dimension ref="A1:AX2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18171,7 +18518,7 @@
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18212,7 +18559,7 @@
 </file>
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18262,7 +18609,7 @@
 </file>
 
 <file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18337,7 +18684,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="K4">
         <v>20019933</v>
@@ -18350,7 +18697,7 @@
 </file>
 
 <file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18418,11 +18765,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -18749,7 +19097,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -18765,7 +19113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4500-000000000000}">
   <dimension ref="A1:AM5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18970,19 +19318,19 @@
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B5" t="s">
         <v>1461</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1462</v>
       </c>
       <c r="C5" t="s">
         <v>1173</v>
       </c>
       <c r="D5" t="s">
-        <v>1547</v>
+        <v>1583</v>
       </c>
       <c r="E5" t="s">
-        <v>1548</v>
+        <v>1584</v>
       </c>
       <c r="F5" t="s">
         <v>1116</v>
@@ -18991,25 +19339,25 @@
         <v>1118</v>
       </c>
       <c r="H5" t="s">
-        <v>1549</v>
+        <v>1585</v>
       </c>
       <c r="I5" t="s">
         <v>1121</v>
       </c>
       <c r="J5" t="s">
-        <v>1550</v>
+        <v>1586</v>
       </c>
       <c r="K5" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="L5" t="s">
         <v>1178</v>
       </c>
       <c r="M5" t="s">
-        <v>1551</v>
+        <v>1587</v>
       </c>
       <c r="N5" t="s">
-        <v>1552</v>
+        <v>1588</v>
       </c>
       <c r="O5" t="s">
         <v>1116</v>
@@ -19018,19 +19366,19 @@
         <v>1118</v>
       </c>
       <c r="Q5" t="s">
-        <v>1553</v>
+        <v>1589</v>
       </c>
       <c r="R5" t="s">
         <v>1121</v>
       </c>
       <c r="S5" t="s">
-        <v>1554</v>
+        <v>1590</v>
       </c>
       <c r="T5" t="s">
         <v>201</v>
       </c>
       <c r="U5" t="s">
-        <v>1555</v>
+        <v>1591</v>
       </c>
       <c r="V5" t="s">
         <v>1118</v>
@@ -19094,10 +19442,10 @@
 </file>
 
 <file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4600-000000000000}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -19116,7 +19464,7 @@
         <v>208</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>1585</v>
+        <v>1571</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>109</v>
@@ -19184,10 +19532,10 @@
         <v>2001</v>
       </c>
       <c r="B2" t="s">
-        <v>1478</v>
+        <v>1597</v>
       </c>
       <c r="C2" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="D2" t="s">
         <v>1178</v>
@@ -19249,11 +19597,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -19397,7 +19746,7 @@
 </file>
 
 <file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4800-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -19541,7 +19890,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -19557,7 +19906,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>

</xml_diff>